<commit_message>
More work and tests on ACAerodynamicAndStabilityManager.
</commit_message>
<xml_diff>
--- a/JPADSandBox_v2/out/ATR-72/AERODYNAMIC_AND_STABILITY_CRUISE/Aerodynamic_and_Stability_CRUISE.xlsx
+++ b/JPADSandBox_v2/out/ATR-72/AERODYNAMIC_AND_STABILITY_CRUISE/Aerodynamic_and_Stability_CRUISE.xlsx
@@ -10,12 +10,13 @@
     <sheet name="HORIZONTAL_TAIL" r:id="rId4" sheetId="2"/>
     <sheet name="VERTICAL_TAIL" r:id="rId5" sheetId="3"/>
     <sheet name="FUSELAGE" r:id="rId6" sheetId="4"/>
+    <sheet name="NACELLE" r:id="rId7" sheetId="5"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="814" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="851" uniqueCount="114">
   <si>
     <t>Description</t>
   </si>
@@ -33155,7 +33156,7 @@
         <v>5</v>
       </c>
       <c r="C18" t="n">
-        <v>-0.017440525689364335</v>
+        <v>-0.08758897794946623</v>
       </c>
     </row>
     <row r="19">
@@ -33412,6 +33413,707 @@
     </row>
     <row r="25">
       <c r="A25" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="35"/>
+  <cols>
+    <col min="2" max="2" width="8.0" customWidth="true"/>
+    <col min="3" max="3" width="15.0" customWidth="true"/>
+    <col min="4" max="4" width="15.0" customWidth="true"/>
+    <col min="5" max="5" width="15.0" customWidth="true"/>
+    <col min="6" max="6" width="15.0" customWidth="true"/>
+    <col min="7" max="7" width="15.0" customWidth="true"/>
+    <col min="8" max="8" width="15.0" customWidth="true"/>
+    <col min="9" max="9" width="15.0" customWidth="true"/>
+    <col min="10" max="10" width="15.0" customWidth="true"/>
+    <col min="11" max="11" width="15.0" customWidth="true"/>
+    <col min="12" max="12" width="15.0" customWidth="true"/>
+    <col min="13" max="13" width="15.0" customWidth="true"/>
+    <col min="14" max="14" width="15.0" customWidth="true"/>
+    <col min="15" max="15" width="15.0" customWidth="true"/>
+    <col min="16" max="16" width="15.0" customWidth="true"/>
+    <col min="17" max="17" width="15.0" customWidth="true"/>
+    <col min="18" max="18" width="15.0" customWidth="true"/>
+    <col min="19" max="19" width="15.0" customWidth="true"/>
+    <col min="20" max="20" width="15.0" customWidth="true"/>
+    <col min="21" max="21" width="15.0" customWidth="true"/>
+    <col min="22" max="22" width="15.0" customWidth="true"/>
+    <col min="23" max="23" width="15.0" customWidth="true"/>
+    <col min="24" max="24" width="15.0" customWidth="true"/>
+    <col min="25" max="25" width="15.0" customWidth="true"/>
+    <col min="26" max="26" width="15.0" customWidth="true"/>
+    <col min="27" max="27" width="15.0" customWidth="true"/>
+    <col min="28" max="28" width="15.0" customWidth="true"/>
+    <col min="29" max="29" width="15.0" customWidth="true"/>
+    <col min="30" max="30" width="15.0" customWidth="true"/>
+    <col min="31" max="31" width="15.0" customWidth="true"/>
+    <col min="32" max="32" width="15.0" customWidth="true"/>
+    <col min="33" max="33" width="15.0" customWidth="true"/>
+    <col min="34" max="34" width="15.0" customWidth="true"/>
+    <col min="35" max="35" width="15.0" customWidth="true"/>
+    <col min="36" max="36" width="15.0" customWidth="true"/>
+    <col min="37" max="37" width="15.0" customWidth="true"/>
+    <col min="38" max="38" width="15.0" customWidth="true"/>
+    <col min="39" max="39" width="15.0" customWidth="true"/>
+    <col min="40" max="40" width="15.0" customWidth="true"/>
+    <col min="41" max="41" width="15.0" customWidth="true"/>
+    <col min="42" max="42" width="15.0" customWidth="true"/>
+    <col min="43" max="43" width="15.0" customWidth="true"/>
+    <col min="44" max="44" width="15.0" customWidth="true"/>
+    <col min="45" max="45" width="15.0" customWidth="true"/>
+    <col min="46" max="46" width="15.0" customWidth="true"/>
+    <col min="47" max="47" width="15.0" customWidth="true"/>
+    <col min="48" max="48" width="15.0" customWidth="true"/>
+    <col min="49" max="49" width="15.0" customWidth="true"/>
+    <col min="50" max="50" width="15.0" customWidth="true"/>
+    <col min="51" max="51" width="15.0" customWidth="true"/>
+    <col min="52" max="52" width="15.0" customWidth="true"/>
+    <col min="53" max="53" width="15.0" customWidth="true"/>
+    <col min="54" max="54" width="15.0" customWidth="true"/>
+    <col min="55" max="55" width="15.0" customWidth="true"/>
+    <col min="56" max="56" width="15.0" customWidth="true"/>
+    <col min="57" max="57" width="15.0" customWidth="true"/>
+    <col min="58" max="58" width="15.0" customWidth="true"/>
+    <col min="59" max="59" width="15.0" customWidth="true"/>
+    <col min="60" max="60" width="15.0" customWidth="true"/>
+    <col min="61" max="61" width="15.0" customWidth="true"/>
+    <col min="62" max="62" width="15.0" customWidth="true"/>
+    <col min="63" max="63" width="15.0" customWidth="true"/>
+    <col min="64" max="64" width="15.0" customWidth="true"/>
+    <col min="65" max="65" width="15.0" customWidth="true"/>
+    <col min="66" max="66" width="15.0" customWidth="true"/>
+    <col min="67" max="67" width="15.0" customWidth="true"/>
+    <col min="68" max="68" width="15.0" customWidth="true"/>
+    <col min="69" max="69" width="15.0" customWidth="true"/>
+    <col min="70" max="70" width="15.0" customWidth="true"/>
+    <col min="71" max="71" width="15.0" customWidth="true"/>
+    <col min="72" max="72" width="15.0" customWidth="true"/>
+    <col min="73" max="73" width="15.0" customWidth="true"/>
+    <col min="74" max="74" width="15.0" customWidth="true"/>
+    <col min="75" max="75" width="15.0" customWidth="true"/>
+    <col min="76" max="76" width="15.0" customWidth="true"/>
+    <col min="77" max="77" width="15.0" customWidth="true"/>
+    <col min="78" max="78" width="15.0" customWidth="true"/>
+    <col min="79" max="79" width="15.0" customWidth="true"/>
+    <col min="80" max="80" width="15.0" customWidth="true"/>
+    <col min="81" max="81" width="15.0" customWidth="true"/>
+    <col min="82" max="82" width="15.0" customWidth="true"/>
+    <col min="83" max="83" width="15.0" customWidth="true"/>
+    <col min="84" max="84" width="15.0" customWidth="true"/>
+    <col min="85" max="85" width="15.0" customWidth="true"/>
+    <col min="86" max="86" width="15.0" customWidth="true"/>
+    <col min="87" max="87" width="15.0" customWidth="true"/>
+    <col min="88" max="88" width="15.0" customWidth="true"/>
+    <col min="89" max="89" width="15.0" customWidth="true"/>
+    <col min="90" max="90" width="15.0" customWidth="true"/>
+    <col min="91" max="91" width="15.0" customWidth="true"/>
+    <col min="92" max="92" width="15.0" customWidth="true"/>
+    <col min="93" max="93" width="15.0" customWidth="true"/>
+    <col min="94" max="94" width="15.0" customWidth="true"/>
+    <col min="95" max="95" width="15.0" customWidth="true"/>
+    <col min="96" max="96" width="15.0" customWidth="true"/>
+    <col min="97" max="97" width="15.0" customWidth="true"/>
+    <col min="98" max="98" width="15.0" customWidth="true"/>
+    <col min="99" max="99" width="15.0" customWidth="true"/>
+    <col min="100" max="100" width="15.0" customWidth="true"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>106</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" t="n">
+        <v>0.0011625552958951042</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>107</v>
+      </c>
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" t="n">
+        <v>9.96975407110667E-6</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>110</v>
+      </c>
+      <c r="B5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" t="n">
+        <v>0.001265079381909406</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6"/>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" t="n">
+        <v>0.0036817660153983297</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" t="n">
+        <v>-7.999999999999998</v>
+      </c>
+      <c r="D10" t="n">
+        <v>-6.999999999999998</v>
+      </c>
+      <c r="E10" t="n">
+        <v>-5.999999999999999</v>
+      </c>
+      <c r="F10" t="n">
+        <v>-4.999999999999999</v>
+      </c>
+      <c r="G10" t="n">
+        <v>-3.999999999999999</v>
+      </c>
+      <c r="H10" t="n">
+        <v>-2.999999999999999</v>
+      </c>
+      <c r="I10" t="n">
+        <v>-1.9999999999999996</v>
+      </c>
+      <c r="J10" t="n">
+        <v>-0.9999999999999998</v>
+      </c>
+      <c r="K10" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="L10" t="n">
+        <v>0.9999999999999998</v>
+      </c>
+      <c r="M10" t="n">
+        <v>1.9999999999999998</v>
+      </c>
+      <c r="N10" t="n">
+        <v>2.9999999999999996</v>
+      </c>
+      <c r="O10" t="n">
+        <v>3.9999999999999996</v>
+      </c>
+      <c r="P10" t="n">
+        <v>4.999999999999999</v>
+      </c>
+      <c r="Q10" t="n">
+        <v>5.999999999999999</v>
+      </c>
+      <c r="R10" t="n">
+        <v>6.999999999999999</v>
+      </c>
+      <c r="S10" t="n">
+        <v>7.999999999999999</v>
+      </c>
+      <c r="T10" t="n">
+        <v>8.999999999999998</v>
+      </c>
+      <c r="U10" t="n">
+        <v>9.999999999999998</v>
+      </c>
+      <c r="V10" t="n">
+        <v>10.999999999999998</v>
+      </c>
+      <c r="W10" t="n">
+        <v>11.999999999999998</v>
+      </c>
+      <c r="X10" t="n">
+        <v>12.999999999999998</v>
+      </c>
+      <c r="Y10" t="n">
+        <v>13.999999999999998</v>
+      </c>
+      <c r="Z10" t="n">
+        <v>14.999999999999998</v>
+      </c>
+      <c r="AA10" t="n">
+        <v>15.999999999999998</v>
+      </c>
+      <c r="AB10" t="n">
+        <v>16.999999999999996</v>
+      </c>
+      <c r="AC10" t="n">
+        <v>17.999999999999996</v>
+      </c>
+      <c r="AD10" t="n">
+        <v>18.999999999999996</v>
+      </c>
+      <c r="AE10" t="n">
+        <v>19.999999999999996</v>
+      </c>
+      <c r="AF10" t="n">
+        <v>20.999999999999996</v>
+      </c>
+      <c r="AG10" t="n">
+        <v>21.999999999999996</v>
+      </c>
+      <c r="AH10" t="n">
+        <v>22.999999999999996</v>
+      </c>
+      <c r="AI10" t="n">
+        <v>23.999999999999996</v>
+      </c>
+      <c r="AJ10" t="n">
+        <v>24.999999999999996</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>49</v>
+      </c>
+      <c r="B11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" t="n">
+        <v>0.010711629953751833</v>
+      </c>
+      <c r="D11" t="n">
+        <v>0.008511643624600678</v>
+      </c>
+      <c r="E11" t="n">
+        <v>0.00659940745001889</v>
+      </c>
+      <c r="F11" t="n">
+        <v>0.0049766417109604775</v>
+      </c>
+      <c r="G11" t="n">
+        <v>0.003645066688379452</v>
+      </c>
+      <c r="H11" t="n">
+        <v>0.0026064026632298216</v>
+      </c>
+      <c r="I11" t="n">
+        <v>0.0018623699164655972</v>
+      </c>
+      <c r="J11" t="n">
+        <v>0.0014146887290407888</v>
+      </c>
+      <c r="K11" t="n">
+        <v>0.001265079381909406</v>
+      </c>
+      <c r="L11" t="n">
+        <v>0.0014152621560254586</v>
+      </c>
+      <c r="M11" t="n">
+        <v>0.001866957332342957</v>
+      </c>
+      <c r="N11" t="n">
+        <v>0.0026218851918159104</v>
+      </c>
+      <c r="O11" t="n">
+        <v>0.0036817660153983297</v>
+      </c>
+      <c r="P11" t="n">
+        <v>0.005048320084044223</v>
+      </c>
+      <c r="Q11" t="n">
+        <v>0.006723267678707602</v>
+      </c>
+      <c r="R11" t="n">
+        <v>0.008708329080342476</v>
+      </c>
+      <c r="S11" t="n">
+        <v>0.011005224569902857</v>
+      </c>
+      <c r="T11" t="n">
+        <v>0.013615674428342746</v>
+      </c>
+      <c r="U11" t="n">
+        <v>0.01654139893661617</v>
+      </c>
+      <c r="V11" t="n">
+        <v>0.019784118375677118</v>
+      </c>
+      <c r="W11" t="n">
+        <v>0.02334555302647962</v>
+      </c>
+      <c r="X11" t="n">
+        <v>0.027227423169977675</v>
+      </c>
+      <c r="Y11" t="n">
+        <v>0.031431449087125286</v>
+      </c>
+      <c r="Z11" t="n">
+        <v>0.03595935105887648</v>
+      </c>
+      <c r="AA11" t="n">
+        <v>0.04081284936618526</v>
+      </c>
+      <c r="AB11" t="n">
+        <v>0.04599366429000563</v>
+      </c>
+      <c r="AC11" t="n">
+        <v>0.05150351611129158</v>
+      </c>
+      <c r="AD11" t="n">
+        <v>0.05734412511099718</v>
+      </c>
+      <c r="AE11" t="n">
+        <v>0.06351721157007639</v>
+      </c>
+      <c r="AF11" t="n">
+        <v>0.07002449576948326</v>
+      </c>
+      <c r="AG11" t="n">
+        <v>0.07686769799017171</v>
+      </c>
+      <c r="AH11" t="n">
+        <v>0.08404853851309586</v>
+      </c>
+      <c r="AI11" t="n">
+        <v>0.09156873761920967</v>
+      </c>
+      <c r="AJ11" t="n">
+        <v>0.09943001558946717</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s">
+        <v>112</v>
+      </c>
+      <c r="B16" t="s">
+        <v>5</v>
+      </c>
+      <c r="C16" t="n">
+        <v>-0.0022290592726745195</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="s">
+        <v>57</v>
+      </c>
+      <c r="B17" t="s">
+        <v>5</v>
+      </c>
+      <c r="C17" t="n">
+        <v>2.5909929515425085E-5</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s">
+        <v>58</v>
+      </c>
+      <c r="B18" t="s">
+        <v>5</v>
+      </c>
+      <c r="C18" t="n">
+        <v>-0.0021772394136436693</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="s">
+        <v>21</v>
+      </c>
+      <c r="B21" t="s">
+        <v>16</v>
+      </c>
+      <c r="C21" t="n">
+        <v>-7.999999999999998</v>
+      </c>
+      <c r="D21" t="n">
+        <v>-6.999999999999998</v>
+      </c>
+      <c r="E21" t="n">
+        <v>-5.999999999999999</v>
+      </c>
+      <c r="F21" t="n">
+        <v>-4.999999999999999</v>
+      </c>
+      <c r="G21" t="n">
+        <v>-3.999999999999999</v>
+      </c>
+      <c r="H21" t="n">
+        <v>-2.999999999999999</v>
+      </c>
+      <c r="I21" t="n">
+        <v>-1.9999999999999996</v>
+      </c>
+      <c r="J21" t="n">
+        <v>-0.9999999999999998</v>
+      </c>
+      <c r="K21" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="L21" t="n">
+        <v>0.9999999999999998</v>
+      </c>
+      <c r="M21" t="n">
+        <v>1.9999999999999998</v>
+      </c>
+      <c r="N21" t="n">
+        <v>2.9999999999999996</v>
+      </c>
+      <c r="O21" t="n">
+        <v>3.9999999999999996</v>
+      </c>
+      <c r="P21" t="n">
+        <v>4.999999999999999</v>
+      </c>
+      <c r="Q21" t="n">
+        <v>5.999999999999999</v>
+      </c>
+      <c r="R21" t="n">
+        <v>6.999999999999999</v>
+      </c>
+      <c r="S21" t="n">
+        <v>7.999999999999999</v>
+      </c>
+      <c r="T21" t="n">
+        <v>8.999999999999998</v>
+      </c>
+      <c r="U21" t="n">
+        <v>9.999999999999998</v>
+      </c>
+      <c r="V21" t="n">
+        <v>10.999999999999998</v>
+      </c>
+      <c r="W21" t="n">
+        <v>11.999999999999998</v>
+      </c>
+      <c r="X21" t="n">
+        <v>12.999999999999998</v>
+      </c>
+      <c r="Y21" t="n">
+        <v>13.999999999999998</v>
+      </c>
+      <c r="Z21" t="n">
+        <v>14.999999999999998</v>
+      </c>
+      <c r="AA21" t="n">
+        <v>15.999999999999998</v>
+      </c>
+      <c r="AB21" t="n">
+        <v>16.999999999999996</v>
+      </c>
+      <c r="AC21" t="n">
+        <v>17.999999999999996</v>
+      </c>
+      <c r="AD21" t="n">
+        <v>18.999999999999996</v>
+      </c>
+      <c r="AE21" t="n">
+        <v>19.999999999999996</v>
+      </c>
+      <c r="AF21" t="n">
+        <v>20.999999999999996</v>
+      </c>
+      <c r="AG21" t="n">
+        <v>21.999999999999996</v>
+      </c>
+      <c r="AH21" t="n">
+        <v>22.999999999999996</v>
+      </c>
+      <c r="AI21" t="n">
+        <v>23.999999999999996</v>
+      </c>
+      <c r="AJ21" t="n">
+        <v>24.999999999999996</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="s">
+        <v>60</v>
+      </c>
+      <c r="B22" t="s">
+        <v>5</v>
+      </c>
+      <c r="C22" t="n">
+        <v>-0.0024363387087979202</v>
+      </c>
+      <c r="D22" t="n">
+        <v>-0.002410428779282495</v>
+      </c>
+      <c r="E22" t="n">
+        <v>-0.00238451884976707</v>
+      </c>
+      <c r="F22" t="n">
+        <v>-0.0023586089202516447</v>
+      </c>
+      <c r="G22" t="n">
+        <v>-0.00233269899073622</v>
+      </c>
+      <c r="H22" t="n">
+        <v>-0.0023067890612207946</v>
+      </c>
+      <c r="I22" t="n">
+        <v>-0.0022808791317053697</v>
+      </c>
+      <c r="J22" t="n">
+        <v>-0.0022549692021899444</v>
+      </c>
+      <c r="K22" t="n">
+        <v>-0.0022290592726745195</v>
+      </c>
+      <c r="L22" t="n">
+        <v>-0.0022031493431590946</v>
+      </c>
+      <c r="M22" t="n">
+        <v>-0.0021772394136436693</v>
+      </c>
+      <c r="N22" t="n">
+        <v>-0.0021513294841282444</v>
+      </c>
+      <c r="O22" t="n">
+        <v>-0.002125419554612819</v>
+      </c>
+      <c r="P22" t="n">
+        <v>-0.0020995096250973943</v>
+      </c>
+      <c r="Q22" t="n">
+        <v>-0.002073599695581969</v>
+      </c>
+      <c r="R22" t="n">
+        <v>-0.002047689766066544</v>
+      </c>
+      <c r="S22" t="n">
+        <v>-0.0020217798365511188</v>
+      </c>
+      <c r="T22" t="n">
+        <v>-0.001995869907035694</v>
+      </c>
+      <c r="U22" t="n">
+        <v>-0.0019699599775202686</v>
+      </c>
+      <c r="V22" t="n">
+        <v>-0.0019440500480048437</v>
+      </c>
+      <c r="W22" t="n">
+        <v>-0.0019181401184894184</v>
+      </c>
+      <c r="X22" t="n">
+        <v>-0.0018922301889739935</v>
+      </c>
+      <c r="Y22" t="n">
+        <v>-0.0018663202594585684</v>
+      </c>
+      <c r="Z22" t="n">
+        <v>-0.0018404103299431433</v>
+      </c>
+      <c r="AA22" t="n">
+        <v>-0.0018145004004277183</v>
+      </c>
+      <c r="AB22" t="n">
+        <v>-0.0017885904709122932</v>
+      </c>
+      <c r="AC22" t="n">
+        <v>-0.001762680541396868</v>
+      </c>
+      <c r="AD22" t="n">
+        <v>-0.001736770611881443</v>
+      </c>
+      <c r="AE22" t="n">
+        <v>-0.0017108606823660179</v>
+      </c>
+      <c r="AF22" t="n">
+        <v>-0.0016849507528505928</v>
+      </c>
+      <c r="AG22" t="n">
+        <v>-0.0016590408233351677</v>
+      </c>
+      <c r="AH22" t="n">
+        <v>-0.0016331308938197426</v>
+      </c>
+      <c r="AI22" t="n">
+        <v>-0.0016072209643043175</v>
+      </c>
+      <c r="AJ22" t="n">
+        <v>-0.0015813110347888924</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
More work on ACAerodynamicAndStabilityManager, plot
</commit_message>
<xml_diff>
--- a/JPADSandBox_v2/out/ATR-72/AERODYNAMIC_AND_STABILITY_CRUISE/Aerodynamic_and_Stability_CRUISE.xlsx
+++ b/JPADSandBox_v2/out/ATR-72/AERODYNAMIC_AND_STABILITY_CRUISE/Aerodynamic_and_Stability_CRUISE.xlsx
@@ -32893,7 +32893,7 @@
         <v>5</v>
       </c>
       <c r="C8" t="n">
-        <v>2.3907597433886919E-4</v>
+        <v>2.4409826849042238E-4</v>
       </c>
     </row>
     <row r="9">
@@ -32904,7 +32904,7 @@
         <v>5</v>
       </c>
       <c r="C9" t="n">
-        <v>0.007764789288208396</v>
+        <v>0.007769811582359949</v>
       </c>
     </row>
     <row r="10">
@@ -33035,106 +33035,106 @@
         <v>5</v>
       </c>
       <c r="C13" t="n">
-        <v>0.010758594167941888</v>
+        <v>0.009973772233345755</v>
       </c>
       <c r="D13" t="n">
-        <v>0.010385959212082702</v>
+        <v>0.009830412864635183</v>
       </c>
       <c r="E13" t="n">
-        <v>0.00996443339393489</v>
+        <v>0.00958479437032612</v>
       </c>
       <c r="F13" t="n">
-        <v>0.009521541488445433</v>
+        <v>0.009273573382526497</v>
       </c>
       <c r="G13" t="n">
-        <v>0.009081309772405967</v>
+        <v>0.008928747343212536</v>
       </c>
       <c r="H13" t="n">
-        <v>0.008664804768663078</v>
+        <v>0.008578371986873187</v>
       </c>
       <c r="I13" t="n">
-        <v>0.008290621301139566</v>
+        <v>0.008247211316882243</v>
       </c>
       <c r="J13" t="n">
-        <v>0.007975320956007007</v>
+        <v>0.007957321534337976</v>
       </c>
       <c r="K13" t="n">
-        <v>0.0077338224761858455</v>
+        <v>0.007728570953215742</v>
       </c>
       <c r="L13" t="n">
-        <v>0.007579745992354634</v>
+        <v>0.007579098436431128</v>
       </c>
       <c r="M13" t="n">
         <v>0.007525713313869527</v>
       </c>
       <c r="N13" t="n">
-        <v>0.007583606768123509</v>
+        <v>0.007584240096527658</v>
       </c>
       <c r="O13" t="n">
-        <v>0.007764789288208396</v>
+        <v>0.007769811582359949</v>
       </c>
       <c r="P13" t="n">
-        <v>0.008080288608125286</v>
+        <v>0.008097114161683527</v>
       </c>
       <c r="Q13" t="n">
-        <v>0.008540948534555512</v>
+        <v>0.008580589276178944</v>
       </c>
       <c r="R13" t="n">
-        <v>0.00915755032711915</v>
+        <v>0.009234595069312023</v>
       </c>
       <c r="S13" t="n">
-        <v>0.009940907238245674</v>
+        <v>0.01007353229156886</v>
       </c>
       <c r="T13" t="n">
-        <v>0.010901935242700767</v>
+        <v>0.011111938495821587</v>
       </c>
       <c r="U13" t="n">
-        <v>0.01205170292913712</v>
+        <v>0.012364554481331134</v>
       </c>
       <c r="V13" t="n">
-        <v>0.01340146343562804</v>
+        <v>0.013846366824489408</v>
       </c>
       <c r="W13" t="n">
-        <v>0.014962671191983582</v>
+        <v>0.015572630175710884</v>
       </c>
       <c r="X13" t="n">
-        <v>0.016746986087783487</v>
+        <v>0.01755887281028817</v>
       </c>
       <c r="Y13" t="n">
-        <v>0.018766267520538123</v>
+        <v>0.019820888701919382</v>
       </c>
       <c r="Z13" t="n">
-        <v>0.02103256059720997</v>
+        <v>0.02237471914632719</v>
       </c>
       <c r="AA13" t="n">
-        <v>0.023558076568399453</v>
+        <v>0.025236626704121076</v>
       </c>
       <c r="AB13" t="n">
-        <v>0.026355169371586454</v>
+        <v>0.02842306396182197</v>
       </c>
       <c r="AC13" t="n">
-        <v>0.029436309951507984</v>
+        <v>0.03195063933254655</v>
       </c>
       <c r="AD13" t="n">
-        <v>0.03281405981541598</v>
+        <v>0.03583608183772886</v>
       </c>
       <c r="AE13" t="n">
-        <v>0.03650104507172447</v>
+        <v>0.04009620653260476</v>
       </c>
       <c r="AF13" t="n">
-        <v>0.04050993199528157</v>
+        <v>0.04474788196480744</v>
       </c>
       <c r="AG13" t="n">
-        <v>0.044853404963761424</v>
+        <v>0.04980800079074602</v>
       </c>
       <c r="AH13" t="n">
-        <v>0.04954414741973539</v>
+        <v>0.05529345442148915</v>
       </c>
       <c r="AI13" t="n">
-        <v>0.054594826333808966</v>
+        <v>0.06122111233125784</v>
       </c>
       <c r="AJ13" t="n">
-        <v>0.0600180804774492</v>
+        <v>0.06760780643954489</v>
       </c>
     </row>
     <row r="14">

</xml_diff>

<commit_message>
More work on ACAerodynamicAndStabilityManager.
</commit_message>
<xml_diff>
--- a/JPADSandBox_v2/out/ATR-72/AERODYNAMIC_AND_STABILITY_CRUISE/Aerodynamic_and_Stability_CRUISE.xlsx
+++ b/JPADSandBox_v2/out/ATR-72/AERODYNAMIC_AND_STABILITY_CRUISE/Aerodynamic_and_Stability_CRUISE.xlsx
@@ -35189,106 +35189,106 @@
         <v>5</v>
       </c>
       <c r="C6" t="n">
-        <v>-0.186955579098393</v>
+        <v>-0.2581980580118683</v>
       </c>
       <c r="D6" t="n">
-        <v>-0.10704536974151237</v>
+        <v>-0.1762976077874291</v>
       </c>
       <c r="E6" t="n">
-        <v>-0.027135160384631762</v>
+        <v>-0.09439715756298993</v>
       </c>
       <c r="F6" t="n">
-        <v>0.05277504897224886</v>
+        <v>-0.01249670733855076</v>
       </c>
       <c r="G6" t="n">
-        <v>0.13268525832912947</v>
+        <v>0.06940374288588842</v>
       </c>
       <c r="H6" t="n">
-        <v>0.21259546768601012</v>
+        <v>0.15130419311032758</v>
       </c>
       <c r="I6" t="n">
-        <v>0.29250567704289077</v>
+        <v>0.2332046433347668</v>
       </c>
       <c r="J6" t="n">
-        <v>0.3724158863997713</v>
+        <v>0.3151050935592059</v>
       </c>
       <c r="K6" t="n">
-        <v>0.45232609575665195</v>
+        <v>0.3970055437836451</v>
       </c>
       <c r="L6" t="n">
-        <v>0.5322363051135326</v>
+        <v>0.4789059940080843</v>
       </c>
       <c r="M6" t="n">
-        <v>0.6121465144704132</v>
+        <v>0.5608064442325235</v>
       </c>
       <c r="N6" t="n">
-        <v>0.6920567238272939</v>
+        <v>0.6427068944569627</v>
       </c>
       <c r="O6" t="n">
-        <v>0.7719669331841745</v>
+        <v>0.724607344681402</v>
       </c>
       <c r="P6" t="n">
-        <v>0.8518771425410552</v>
+        <v>0.8065077949058411</v>
       </c>
       <c r="Q6" t="n">
-        <v>0.9317873518979358</v>
+        <v>0.8884082451302804</v>
       </c>
       <c r="R6" t="n">
-        <v>1.0116977685249442</v>
+        <v>0.9703086953547195</v>
       </c>
       <c r="S6" t="n">
-        <v>1.091652804733644</v>
+        <v>1.0522091455791587</v>
       </c>
       <c r="T6" t="n">
-        <v>1.1717721755378383</v>
+        <v>1.1341095958035978</v>
       </c>
       <c r="U6" t="n">
-        <v>1.2521337595591233</v>
+        <v>1.2160157287502524</v>
       </c>
       <c r="V6" t="n">
-        <v>1.3327570725769333</v>
+        <v>1.2980477636752046</v>
       </c>
       <c r="W6" t="n">
-        <v>1.4136032675285373</v>
+        <v>1.3803739193261386</v>
       </c>
       <c r="X6" t="n">
-        <v>1.4945751345090426</v>
+        <v>1.463058094358339</v>
       </c>
       <c r="Y6" t="n">
-        <v>1.575517100771391</v>
+        <v>1.546053678391627</v>
       </c>
       <c r="Z6" t="n">
-        <v>1.6562144627232755</v>
+        <v>1.6292027840072854</v>
       </c>
       <c r="AA6" t="n">
-        <v>1.7339972570348157</v>
+        <v>1.7098401178557248</v>
       </c>
       <c r="AB6" t="n">
-        <v>1.8000823600992957</v>
+        <v>1.7791350801172288</v>
       </c>
       <c r="AC6" t="n">
-        <v>1.8483556970459438</v>
+        <v>1.8308739735147292</v>
       </c>
       <c r="AD6" t="n">
-        <v>1.8772459346488912</v>
+        <v>1.8633336962227653</v>
       </c>
       <c r="AE6" t="n">
-        <v>1.8897244813272143</v>
+        <v>1.8792817418675307</v>
       </c>
       <c r="AF6" t="n">
-        <v>1.8933054871447341</v>
+        <v>1.885976199526664</v>
       </c>
       <c r="AG6" t="n">
-        <v>1.9000458438103294</v>
+        <v>1.8951657537295743</v>
       </c>
       <c r="AH6" t="n">
-        <v>1.926545184677597</v>
+        <v>1.9230896844570884</v>
       </c>
       <c r="AI6" t="n">
-        <v>1.9939458847450218</v>
+        <v>1.9904778671416283</v>
       </c>
       <c r="AJ6" t="n">
-        <v>2.1279330606562032</v>
+        <v>2.1225507726674335</v>
       </c>
     </row>
     <row r="7">
@@ -35419,106 +35419,106 @@
         <v>5</v>
       </c>
       <c r="C10" t="n">
-        <v>-0.42372169672024607</v>
+        <v>0.01937194426159472</v>
       </c>
       <c r="D10" t="n">
-        <v>-0.47508876658973476</v>
+        <v>-0.04434574675545527</v>
       </c>
       <c r="E10" t="n">
-        <v>-0.5264173711346648</v>
+        <v>-0.1080249724479466</v>
       </c>
       <c r="F10" t="n">
-        <v>-0.5777029906096087</v>
+        <v>-0.1716612130704518</v>
       </c>
       <c r="G10" t="n">
-        <v>-0.628953093470086</v>
+        <v>-0.23526193707849027</v>
       </c>
       <c r="H10" t="n">
-        <v>-0.679793851610983</v>
+        <v>-0.2984533163669487</v>
       </c>
       <c r="I10" t="n">
-        <v>-0.7112054673537456</v>
+        <v>-0.3422155532572726</v>
       </c>
       <c r="J10" t="n">
-        <v>-0.7419637848152227</v>
+        <v>-0.38532449186631107</v>
       </c>
       <c r="K10" t="n">
-        <v>-0.7727563767652905</v>
+        <v>-0.42846770496394004</v>
       </c>
       <c r="L10" t="n">
-        <v>-0.8035913219507578</v>
+        <v>-0.47165327129696877</v>
       </c>
       <c r="M10" t="n">
-        <v>-0.8344790930620956</v>
+        <v>-0.514891663555868</v>
       </c>
       <c r="N10" t="n">
-        <v>-0.8654280661516355</v>
+        <v>-0.558191257792969</v>
       </c>
       <c r="O10" t="n">
-        <v>-0.8964464753787877</v>
+        <v>-0.6015602881676829</v>
       </c>
       <c r="P10" t="n">
-        <v>-0.9275420843931991</v>
+        <v>-0.6450065183296554</v>
       </c>
       <c r="Q10" t="n">
-        <v>-0.9587200438185567</v>
+        <v>-0.6885350989025741</v>
       </c>
       <c r="R10" t="n">
-        <v>-0.9899913142390191</v>
+        <v>-0.7321557042369233</v>
       </c>
       <c r="S10" t="n">
-        <v>-1.021640200468171</v>
+        <v>-0.7758770344979522</v>
       </c>
       <c r="T10" t="n">
-        <v>-1.0544144758514915</v>
+        <v>-0.8197039605989457</v>
       </c>
       <c r="U10" t="n">
-        <v>-1.0888044844775735</v>
+        <v>-0.863678808393018</v>
       </c>
       <c r="V10" t="n">
-        <v>-1.1249524515350982</v>
+        <v>-0.9085687276740065</v>
       </c>
       <c r="W10" t="n">
-        <v>-1.1635812311404847</v>
+        <v>-0.9563815383223945</v>
       </c>
       <c r="X10" t="n">
-        <v>-1.2146196208783606</v>
+        <v>-1.0180458117807394</v>
       </c>
       <c r="Y10" t="n">
-        <v>-1.3003065527265145</v>
+        <v>-1.116476655928256</v>
       </c>
       <c r="Z10" t="n">
-        <v>-1.426862485398845</v>
+        <v>-1.2582471074238035</v>
       </c>
       <c r="AA10" t="n">
-        <v>-1.5689573716339889</v>
+        <v>-1.4180560989944608</v>
       </c>
       <c r="AB10" t="n">
-        <v>-1.6366937031995699</v>
+        <v>-1.5057115044398242</v>
       </c>
       <c r="AC10" t="n">
-        <v>-1.67022041685598</v>
+        <v>-1.5607440445957532</v>
       </c>
       <c r="AD10" t="n">
-        <v>-1.600664674284372</v>
+        <v>-1.5133390672623706</v>
       </c>
       <c r="AE10" t="n">
-        <v>-1.5689680497247505</v>
+        <v>-1.503172734842188</v>
       </c>
       <c r="AF10" t="n">
-        <v>-1.563706037902051</v>
+        <v>-1.517231532266118</v>
       </c>
       <c r="AG10" t="n">
-        <v>-1.5386476956628121</v>
+        <v>-1.507371908630233</v>
       </c>
       <c r="AH10" t="n">
-        <v>-1.4908928552461516</v>
+        <v>-1.468457490466656</v>
       </c>
       <c r="AI10" t="n">
-        <v>-1.4178640362369221</v>
+        <v>-1.395350993696765</v>
       </c>
       <c r="AJ10" t="n">
-        <v>-1.3169804660536704</v>
+        <v>-1.28258824411912</v>
       </c>
     </row>
     <row r="11">
@@ -35539,106 +35539,106 @@
         <v>5</v>
       </c>
       <c r="C13" t="n">
-        <v>-0.44260224007413396</v>
+        <v>-0.00663284698364075</v>
       </c>
       <c r="D13" t="n">
-        <v>-0.4860255350921828</v>
+        <v>-0.062207739062495104</v>
       </c>
       <c r="E13" t="n">
-        <v>-0.5293725208493649</v>
+        <v>-0.1177063218804826</v>
       </c>
       <c r="F13" t="n">
-        <v>-0.5726619011822089</v>
+        <v>-0.17314729927413214</v>
       </c>
       <c r="G13" t="n">
-        <v>-0.6159021620773741</v>
+        <v>-0.22853915723010268</v>
       </c>
       <c r="H13" t="n">
-        <v>-0.6587239649252096</v>
+        <v>-0.28351255713874357</v>
       </c>
       <c r="I13" t="n">
-        <v>-0.6821109963790114</v>
+        <v>-0.3190511856533509</v>
       </c>
       <c r="J13" t="n">
-        <v>-0.7048392936572737</v>
+        <v>-0.3539310799924186</v>
       </c>
       <c r="K13" t="n">
-        <v>-0.7275997282340864</v>
+        <v>-0.3888431116300366</v>
       </c>
       <c r="L13" t="n">
-        <v>-0.7504042884585687</v>
+        <v>-0.4237992689153244</v>
       </c>
       <c r="M13" t="n">
-        <v>-0.7732644416150537</v>
+        <v>-0.4588110191326151</v>
       </c>
       <c r="N13" t="n">
-        <v>-0.7961918290709497</v>
+        <v>-0.49389000364931657</v>
       </c>
       <c r="O13" t="n">
-        <v>-0.8191968055827447</v>
+        <v>-0.5290465772219171</v>
       </c>
       <c r="P13" t="n">
-        <v>-0.8422897612201375</v>
+        <v>-0.5642911299201152</v>
       </c>
       <c r="Q13" t="n">
-        <v>-0.8654792889778147</v>
+        <v>-0.5996322547385978</v>
       </c>
       <c r="R13" t="n">
-        <v>-0.8887780546846316</v>
+        <v>-0.6350813519995582</v>
       </c>
       <c r="S13" t="n">
-        <v>-0.912467378862778</v>
+        <v>-0.6706485788080078</v>
       </c>
       <c r="T13" t="n">
-        <v>-0.9372880635413119</v>
+        <v>-0.7063438062621898</v>
       </c>
       <c r="U13" t="n">
-        <v>-0.9637255165888979</v>
+        <v>-0.7422116435852298</v>
       </c>
       <c r="V13" t="n">
-        <v>-0.9919173847021504</v>
+        <v>-0.7790045917312317</v>
       </c>
       <c r="W13" t="n">
-        <v>-1.022598318517076</v>
+        <v>-0.8187215605192255</v>
       </c>
       <c r="X13" t="n">
-        <v>-1.0657100824566927</v>
+        <v>-0.8722879773741419</v>
       </c>
       <c r="Y13" t="n">
-        <v>-1.1435041342935839</v>
+        <v>-0.9626205797333017</v>
       </c>
       <c r="Z13" t="n">
-        <v>-1.2622282485590683</v>
+        <v>-1.0963140384556258</v>
       </c>
       <c r="AA13" t="n">
-        <v>-1.396817679453836</v>
+        <v>-1.2483321207322176</v>
       </c>
       <c r="AB13" t="n">
-        <v>-1.4582198564285207</v>
+        <v>-1.3293323856669819</v>
       </c>
       <c r="AC13" t="n">
-        <v>-1.4872583915624298</v>
+        <v>-1.3795301916553238</v>
       </c>
       <c r="AD13" t="n">
-        <v>-1.415219272242822</v>
+        <v>-1.329284889063433</v>
       </c>
       <c r="AE13" t="n">
-        <v>-1.382777320104259</v>
+        <v>-1.3180262791676642</v>
       </c>
       <c r="AF13" t="n">
-        <v>-1.377709187800224</v>
+        <v>-1.3319676109260976</v>
       </c>
       <c r="AG13" t="n">
-        <v>-1.3526206430596175</v>
+        <v>-1.3218328650351139</v>
       </c>
       <c r="AH13" t="n">
-        <v>-1.303078244194687</v>
+        <v>-1.2809884294372424</v>
       </c>
       <c r="AI13" t="n">
-        <v>-1.2245970360139227</v>
+        <v>-1.2024307952341053</v>
       </c>
       <c r="AJ13" t="n">
-        <v>-1.1123278642550307</v>
+        <v>-1.0784738711193569</v>
       </c>
     </row>
     <row r="14">
@@ -35659,106 +35659,106 @@
         <v>5</v>
       </c>
       <c r="C16" t="n">
-        <v>-0.45770667475724414</v>
+        <v>-0.027436679979828904</v>
       </c>
       <c r="D16" t="n">
-        <v>-0.4947749498941413</v>
+        <v>-0.07649733290812682</v>
       </c>
       <c r="E16" t="n">
-        <v>-0.531736640621125</v>
+        <v>-0.12545140142651134</v>
       </c>
       <c r="F16" t="n">
-        <v>-0.5686290296402894</v>
+        <v>-0.17433616823707637</v>
       </c>
       <c r="G16" t="n">
-        <v>-0.6054614169632049</v>
+        <v>-0.2231609333513927</v>
       </c>
       <c r="H16" t="n">
-        <v>-0.641868055576591</v>
+        <v>-0.2715599497561796</v>
       </c>
       <c r="I16" t="n">
-        <v>-0.6588354195992244</v>
+        <v>-0.30051969157021374</v>
       </c>
       <c r="J16" t="n">
-        <v>-0.6751397007309149</v>
+        <v>-0.32881635049330493</v>
       </c>
       <c r="K16" t="n">
-        <v>-0.6914744094091234</v>
+        <v>-0.3571434369629143</v>
       </c>
       <c r="L16" t="n">
-        <v>-0.7078546616648177</v>
+        <v>-0.38551606701000923</v>
       </c>
       <c r="M16" t="n">
-        <v>-0.7242927204574207</v>
+        <v>-0.41394650359401325</v>
       </c>
       <c r="N16" t="n">
-        <v>-0.740802839406402</v>
+        <v>-0.4424490003343952</v>
       </c>
       <c r="O16" t="n">
-        <v>-0.7573970697459109</v>
+        <v>-0.4710356084653051</v>
       </c>
       <c r="P16" t="n">
-        <v>-0.7740879026816891</v>
+        <v>-0.4997188191924839</v>
       </c>
       <c r="Q16" t="n">
-        <v>-0.7908866851052219</v>
+        <v>-0.5285099794074174</v>
       </c>
       <c r="R16" t="n">
-        <v>-0.8078074470411221</v>
+        <v>-0.5574218702096669</v>
       </c>
       <c r="S16" t="n">
-        <v>-0.8251291215784643</v>
+        <v>-0.5864658142560533</v>
       </c>
       <c r="T16" t="n">
-        <v>-0.8435869336931688</v>
+        <v>-0.6156556827927863</v>
       </c>
       <c r="U16" t="n">
-        <v>-0.8636623422779585</v>
+        <v>-0.6450379117389998</v>
       </c>
       <c r="V16" t="n">
-        <v>-0.8854893312357934</v>
+        <v>-0.675353282977013</v>
       </c>
       <c r="W16" t="n">
-        <v>-0.90981198841835</v>
+        <v>-0.7085935782766912</v>
       </c>
       <c r="X16" t="n">
-        <v>-0.9465824517193595</v>
+        <v>-0.7556817098488651</v>
       </c>
       <c r="Y16" t="n">
-        <v>-1.0180621995472405</v>
+        <v>-0.8395357187773396</v>
       </c>
       <c r="Z16" t="n">
-        <v>-1.1305208590872486</v>
+        <v>-0.9667675832810851</v>
       </c>
       <c r="AA16" t="n">
-        <v>-1.2591059257097152</v>
+        <v>-1.1125529381224237</v>
       </c>
       <c r="AB16" t="n">
-        <v>-1.3154407790116829</v>
+        <v>-1.1882290906487092</v>
       </c>
       <c r="AC16" t="n">
-        <v>-1.340888771327591</v>
+        <v>-1.2345591093029822</v>
       </c>
       <c r="AD16" t="n">
-        <v>-1.2668629506095834</v>
+        <v>-1.1820415465042842</v>
       </c>
       <c r="AE16" t="n">
-        <v>-1.2338247364078667</v>
+        <v>-1.1699091146280465</v>
       </c>
       <c r="AF16" t="n">
-        <v>-1.2289117077187637</v>
+        <v>-1.183756473854083</v>
       </c>
       <c r="AG16" t="n">
-        <v>-1.2037990009770634</v>
+        <v>-1.1734016301590207</v>
       </c>
       <c r="AH16" t="n">
-        <v>-1.1528265553535164</v>
+        <v>-1.1310131806137127</v>
       </c>
       <c r="AI16" t="n">
-        <v>-1.0699834358355256</v>
+        <v>-1.0480946364639787</v>
       </c>
       <c r="AJ16" t="n">
-        <v>-0.9486057828161205</v>
+        <v>-0.9151823727195485</v>
       </c>
     </row>
     <row r="17">
@@ -35784,106 +35784,106 @@
         <v>5</v>
       </c>
       <c r="C20" t="n">
-        <v>-0.1520759780249906</v>
+        <v>-0.2930776590852707</v>
       </c>
       <c r="D20" t="n">
-        <v>-0.0729983496577026</v>
+        <v>-0.21034462787123887</v>
       </c>
       <c r="E20" t="n">
-        <v>0.006079278709585363</v>
+        <v>-0.12761159665720706</v>
       </c>
       <c r="F20" t="n">
-        <v>0.08515690707687332</v>
+        <v>-0.04487856544317523</v>
       </c>
       <c r="G20" t="n">
-        <v>0.16423453544416128</v>
+        <v>0.037854465770856605</v>
       </c>
       <c r="H20" t="n">
-        <v>0.24331216381144927</v>
+        <v>0.12058749698488842</v>
       </c>
       <c r="I20" t="n">
-        <v>0.32238979217873726</v>
+        <v>0.20332052819892027</v>
       </c>
       <c r="J20" t="n">
-        <v>0.40146742054602513</v>
+        <v>0.286053559412952</v>
       </c>
       <c r="K20" t="n">
-        <v>0.4805450489133132</v>
+        <v>0.3687865906269839</v>
       </c>
       <c r="L20" t="n">
-        <v>0.5596226772806011</v>
+        <v>0.45151962184101574</v>
       </c>
       <c r="M20" t="n">
-        <v>0.6387003056478892</v>
+        <v>0.5342526530550475</v>
       </c>
       <c r="N20" t="n">
-        <v>0.7177779340151771</v>
+        <v>0.6169856842690794</v>
       </c>
       <c r="O20" t="n">
-        <v>0.7968555623824652</v>
+        <v>0.6997187154831113</v>
       </c>
       <c r="P20" t="n">
-        <v>0.8759331907497532</v>
+        <v>0.7824517466971431</v>
       </c>
       <c r="Q20" t="n">
-        <v>0.9550151212034692</v>
+        <v>0.865184777911175</v>
       </c>
       <c r="R20" t="n">
-        <v>1.0341696177367081</v>
+        <v>0.9479178091252067</v>
       </c>
       <c r="S20" t="n">
-        <v>1.1134896977213764</v>
+        <v>1.0306508403392387</v>
       </c>
       <c r="T20" t="n">
-        <v>1.1930267516051387</v>
+        <v>1.1133838715532705</v>
       </c>
       <c r="U20" t="n">
-        <v>1.2727886784794045</v>
+        <v>1.1961169027673022</v>
       </c>
       <c r="V20" t="n">
-        <v>1.3527398860793294</v>
+        <v>1.2788627662688565</v>
       </c>
       <c r="W20" t="n">
-        <v>1.4328012907838146</v>
+        <v>1.3617848143917655</v>
       </c>
       <c r="X20" t="n">
-        <v>1.5128503176155064</v>
+        <v>1.4450628695449468</v>
       </c>
       <c r="Y20" t="n">
-        <v>1.592720900240796</v>
+        <v>1.5287402231274478</v>
       </c>
       <c r="Z20" t="n">
-        <v>1.6722027129667345</v>
+        <v>1.6127197201473424</v>
       </c>
       <c r="AA20" t="n">
-        <v>1.7486450418487072</v>
+        <v>1.6943676303294166</v>
       </c>
       <c r="AB20" t="n">
-        <v>1.8132988841511732</v>
+        <v>1.7648557475759015</v>
       </c>
       <c r="AC20" t="n">
-        <v>1.8600991573604466</v>
+        <v>1.8179435989792627</v>
       </c>
       <c r="AD20" t="n">
-        <v>1.8875383920936508</v>
+        <v>1.851852137731134</v>
       </c>
       <c r="AE20" t="n">
-        <v>1.8986667320987636</v>
+        <v>1.8692637431223924</v>
       </c>
       <c r="AF20" t="n">
-        <v>1.901091934254417</v>
+        <v>1.877322220542934</v>
       </c>
       <c r="AG20" t="n">
-        <v>1.9069793685702103</v>
+        <v>1.8876328014819936</v>
       </c>
       <c r="AH20" t="n">
-        <v>1.9330520181863684</v>
+        <v>1.9162621435278129</v>
       </c>
       <c r="AI20" t="n">
-        <v>2.0005904793739133</v>
+        <v>1.9837383303677947</v>
       </c>
       <c r="AJ20" t="n">
-        <v>2.135432961534891</v>
+        <v>2.1150508717887404</v>
       </c>
     </row>
     <row r="21">
@@ -36014,106 +36014,106 @@
         <v>5</v>
       </c>
       <c r="C24" t="n">
-        <v>-0.6411452281280793</v>
+        <v>0.23759067354238889</v>
       </c>
       <c r="D24" t="n">
-        <v>-0.6873456407628913</v>
+        <v>0.1687063252906622</v>
       </c>
       <c r="E24" t="n">
-        <v>-0.7335075880731448</v>
+        <v>0.09986044236349423</v>
       </c>
       <c r="F24" t="n">
-        <v>-0.7796265503134121</v>
+        <v>0.031057544506312373</v>
       </c>
       <c r="G24" t="n">
-        <v>-0.8257099959392126</v>
+        <v>-0.03770983673640271</v>
       </c>
       <c r="H24" t="n">
-        <v>-0.871384096845433</v>
+        <v>-0.10606787325953773</v>
       </c>
       <c r="I24" t="n">
-        <v>-0.8976290553535191</v>
+        <v>-0.1549967673845382</v>
       </c>
       <c r="J24" t="n">
-        <v>-0.9232207155803195</v>
+        <v>-0.2032723632282533</v>
       </c>
       <c r="K24" t="n">
-        <v>-0.9488466502957108</v>
+        <v>-0.2515822335605589</v>
       </c>
       <c r="L24" t="n">
-        <v>-0.9745149382465013</v>
+        <v>-0.29993445712826416</v>
       </c>
       <c r="M24" t="n">
-        <v>-1.0002360521231628</v>
+        <v>-0.3483395066218401</v>
       </c>
       <c r="N24" t="n">
-        <v>-1.0260183679780257</v>
+        <v>-0.39680575809361746</v>
       </c>
       <c r="O24" t="n">
-        <v>-1.051870119970502</v>
+        <v>-0.44534144570300793</v>
       </c>
       <c r="P24" t="n">
-        <v>-1.0777990717502364</v>
+        <v>-0.4939543330996573</v>
       </c>
       <c r="Q24" t="n">
-        <v>-1.103837070930454</v>
+        <v>-0.5426495709072526</v>
       </c>
       <c r="R24" t="n">
-        <v>-1.1304174102942</v>
+        <v>-0.5914368334762785</v>
       </c>
       <c r="S24" t="n">
-        <v>-1.1581260177881876</v>
+        <v>-0.640324820971984</v>
       </c>
       <c r="T24" t="n">
-        <v>-1.1872866724337854</v>
+        <v>-0.6893184043076541</v>
       </c>
       <c r="U24" t="n">
-        <v>-1.217955453965206</v>
+        <v>-0.7384246446856193</v>
       </c>
       <c r="V24" t="n">
-        <v>-1.249932609578332</v>
+        <v>-0.787744292276192</v>
       </c>
       <c r="W24" t="n">
-        <v>-1.283691301758394</v>
+        <v>-0.8392549679850408</v>
       </c>
       <c r="X24" t="n">
-        <v>-1.3290029228204088</v>
+        <v>-0.9046046186762953</v>
       </c>
       <c r="Y24" t="n">
-        <v>-1.4080412858341576</v>
+        <v>-1.007266245916213</v>
       </c>
       <c r="Z24" t="n">
-        <v>-1.527054016967123</v>
+        <v>-1.15418976697489</v>
       </c>
       <c r="AA24" t="n">
-        <v>-1.660830522773118</v>
+        <v>-1.320269982114947</v>
       </c>
       <c r="AB24" t="n">
-        <v>-1.719685035196534</v>
+        <v>-1.4153296195957519</v>
       </c>
       <c r="AC24" t="n">
-        <v>-1.7440705175361315</v>
+        <v>-1.4787332416372576</v>
       </c>
       <c r="AD24" t="n">
-        <v>-1.6655104443730169</v>
+        <v>-1.4403190243478443</v>
       </c>
       <c r="AE24" t="n">
-        <v>-1.6254349892087436</v>
+        <v>-1.4392349453626077</v>
       </c>
       <c r="AF24" t="n">
-        <v>-1.6130005323913914</v>
+        <v>-1.4617582917692986</v>
       </c>
       <c r="AG24" t="n">
-        <v>-1.5826493027522386</v>
+        <v>-1.4588553017450288</v>
       </c>
       <c r="AH24" t="n">
-        <v>-1.532246590876735</v>
+        <v>-1.4243183778272994</v>
       </c>
       <c r="AI24" t="n">
-        <v>-1.460072661057655</v>
+        <v>-1.351757998867062</v>
       </c>
       <c r="AJ24" t="n">
-        <v>-1.3644967717830632</v>
+        <v>-1.2342767405167356</v>
       </c>
     </row>
     <row r="25">
@@ -36134,106 +36134,106 @@
         <v>5</v>
       </c>
       <c r="C27" t="n">
-        <v>-0.656537811374627</v>
+        <v>0.20809792218981316</v>
       </c>
       <c r="D27" t="n">
-        <v>-0.6948777072569585</v>
+        <v>0.14743963097524138</v>
       </c>
       <c r="E27" t="n">
-        <v>-0.7331412938784232</v>
+        <v>0.08685764902153648</v>
       </c>
       <c r="F27" t="n">
-        <v>-0.77134727507555</v>
+        <v>0.0263332724921696</v>
       </c>
       <c r="G27" t="n">
-        <v>-0.8095041368349978</v>
+        <v>-0.03414198459951828</v>
       </c>
       <c r="H27" t="n">
-        <v>-0.8472425405471158</v>
+        <v>-0.09419878364387654</v>
       </c>
       <c r="I27" t="n">
-        <v>-0.8655461728652003</v>
+        <v>-0.13482081129420118</v>
       </c>
       <c r="J27" t="n">
-        <v>-0.8831910710077451</v>
+        <v>-0.17478410476898626</v>
       </c>
       <c r="K27" t="n">
-        <v>-0.9008681064488404</v>
+        <v>-0.21477953554232165</v>
       </c>
       <c r="L27" t="n">
-        <v>-0.9185892675376053</v>
+        <v>-0.25481909196332664</v>
       </c>
       <c r="M27" t="n">
-        <v>-0.9363660215583732</v>
+        <v>-0.2949142413163347</v>
       </c>
       <c r="N27" t="n">
-        <v>-0.9542100098785519</v>
+        <v>-0.33507662496875346</v>
       </c>
       <c r="O27" t="n">
-        <v>-0.9721315872546298</v>
+        <v>-0.37531659767707115</v>
       </c>
       <c r="P27" t="n">
-        <v>-0.9901411437563054</v>
+        <v>-0.41564454951098695</v>
       </c>
       <c r="Q27" t="n">
-        <v>-1.0082735391591584</v>
+        <v>-0.45606907346518666</v>
       </c>
       <c r="R27" t="n">
-        <v>-1.026956965818636</v>
+        <v>-0.49660156986186454</v>
       </c>
       <c r="S27" t="n">
-        <v>-1.0467695068840213</v>
+        <v>-0.5372521958060317</v>
       </c>
       <c r="T27" t="n">
-        <v>-1.0680348025168758</v>
+        <v>-0.578030822395931</v>
       </c>
       <c r="U27" t="n">
-        <v>-1.0908109941845021</v>
+        <v>-0.6189473624761259</v>
       </c>
       <c r="V27" t="n">
-        <v>-1.114899261395145</v>
+        <v>-0.6600986560740519</v>
       </c>
       <c r="W27" t="n">
-        <v>-1.1407885868094574</v>
+        <v>-0.7034539006753091</v>
       </c>
       <c r="X27" t="n">
-        <v>-1.1782658660880945</v>
+        <v>-0.7606463067510372</v>
       </c>
       <c r="Y27" t="n">
-        <v>-1.2495184874542864</v>
+        <v>-0.8551415152476766</v>
       </c>
       <c r="Z27" t="n">
-        <v>-1.3608209551030008</v>
+        <v>-0.9939050043927067</v>
       </c>
       <c r="AA27" t="n">
-        <v>-1.487226052111576</v>
+        <v>-1.1520932526053345</v>
       </c>
       <c r="AB27" t="n">
-        <v>-1.539889536020297</v>
+        <v>-1.2403784340770425</v>
       </c>
       <c r="AC27" t="n">
-        <v>-1.559934146211131</v>
+        <v>-1.2988124261503753</v>
       </c>
       <c r="AD27" t="n">
-        <v>-1.4790357965869907</v>
+        <v>-1.2574130019980698</v>
       </c>
       <c r="AE27" t="n">
-        <v>-1.4383500345110969</v>
+        <v>-1.255090289562598</v>
       </c>
       <c r="AF27" t="n">
-        <v>-1.4262250375785959</v>
+        <v>-1.2773597683276512</v>
       </c>
       <c r="AG27" t="n">
-        <v>-1.395928897673056</v>
+        <v>-1.2740695533746682</v>
       </c>
       <c r="AH27" t="n">
-        <v>-1.3437812964743931</v>
+        <v>-1.2375320708908129</v>
       </c>
       <c r="AI27" t="n">
-        <v>-1.2661412013717666</v>
+        <v>-1.159511754081786</v>
       </c>
       <c r="AJ27" t="n">
-        <v>-1.1590941798965546</v>
+        <v>-1.030912357604842</v>
       </c>
     </row>
     <row r="28">
@@ -36254,106 +36254,106 @@
         <v>5</v>
       </c>
       <c r="C30" t="n">
-        <v>-0.6688518779718648</v>
+        <v>0.18450372110775265</v>
       </c>
       <c r="D30" t="n">
-        <v>-0.7009033604522121</v>
+        <v>0.13042627552290492</v>
       </c>
       <c r="E30" t="n">
-        <v>-0.7328482585226459</v>
+        <v>0.07645541434797043</v>
       </c>
       <c r="F30" t="n">
-        <v>-0.7647238548852603</v>
+        <v>0.022553854880855373</v>
       </c>
       <c r="G30" t="n">
-        <v>-0.796539449551626</v>
+        <v>-0.03128770289001087</v>
       </c>
       <c r="H30" t="n">
-        <v>-0.8279292955084621</v>
+        <v>-0.08470351195134768</v>
       </c>
       <c r="I30" t="n">
-        <v>-0.8398798668745455</v>
+        <v>-0.11868004642193179</v>
       </c>
       <c r="J30" t="n">
-        <v>-0.851167355349686</v>
+        <v>-0.1519934980015729</v>
       </c>
       <c r="K30" t="n">
-        <v>-0.8624852713713447</v>
+        <v>-0.18533737712773218</v>
       </c>
       <c r="L30" t="n">
-        <v>-0.8738487309704888</v>
+        <v>-0.21872679983137702</v>
       </c>
       <c r="M30" t="n">
-        <v>-0.8852699971065421</v>
+        <v>-0.252174029071931</v>
       </c>
       <c r="N30" t="n">
-        <v>-0.8967633233989735</v>
+        <v>-0.28569331846886276</v>
       </c>
       <c r="O30" t="n">
-        <v>-0.9083407610819326</v>
+        <v>-0.3192967192563224</v>
       </c>
       <c r="P30" t="n">
-        <v>-0.9200148013611609</v>
+        <v>-0.3529967226400514</v>
       </c>
       <c r="Q30" t="n">
-        <v>-0.9318227137421229</v>
+        <v>-0.38680467551153475</v>
       </c>
       <c r="R30" t="n">
-        <v>-0.9441886102381856</v>
+        <v>-0.4207333589703343</v>
       </c>
       <c r="S30" t="n">
-        <v>-0.9576842981606889</v>
+        <v>-0.45479409567327045</v>
       </c>
       <c r="T30" t="n">
-        <v>-0.9726333065833489</v>
+        <v>-0.48900075686655353</v>
       </c>
       <c r="U30" t="n">
-        <v>-0.9890954263599402</v>
+        <v>-0.5233655367085323</v>
       </c>
       <c r="V30" t="n">
-        <v>-1.006872582848596</v>
+        <v>-0.5579821471123412</v>
       </c>
       <c r="W30" t="n">
-        <v>-1.0264664148503093</v>
+        <v>-0.5948130468275248</v>
       </c>
       <c r="X30" t="n">
-        <v>-1.0576762207022445</v>
+        <v>-0.6454796572108317</v>
       </c>
       <c r="Y30" t="n">
-        <v>-1.1227002487503908</v>
+        <v>-0.7334417307128489</v>
       </c>
       <c r="Z30" t="n">
-        <v>-1.227834505611704</v>
+        <v>-0.8656771943269612</v>
       </c>
       <c r="AA30" t="n">
-        <v>-1.3483424755823443</v>
+        <v>-1.0175518689976457</v>
       </c>
       <c r="AB30" t="n">
-        <v>-1.396053136679309</v>
+        <v>-1.1004174856620756</v>
       </c>
       <c r="AC30" t="n">
-        <v>-1.412625049151132</v>
+        <v>-1.1548757737608708</v>
       </c>
       <c r="AD30" t="n">
-        <v>-1.3298560783581717</v>
+        <v>-1.1110881841182518</v>
       </c>
       <c r="AE30" t="n">
-        <v>-1.288682070752981</v>
+        <v>-1.1077745649225914</v>
       </c>
       <c r="AF30" t="n">
-        <v>-1.2768046417283605</v>
+        <v>-1.129840949574335</v>
       </c>
       <c r="AG30" t="n">
-        <v>-1.2465525736097116</v>
+        <v>-1.126240954678381</v>
       </c>
       <c r="AH30" t="n">
-        <v>-1.1930090609525208</v>
+        <v>-1.0881030253416255</v>
       </c>
       <c r="AI30" t="n">
-        <v>-1.1109960336230578</v>
+        <v>-1.0057147582535668</v>
       </c>
       <c r="AJ30" t="n">
-        <v>-0.9947721063873496</v>
+        <v>-0.8682208512753289</v>
       </c>
     </row>
     <row r="31">
@@ -36379,106 +36379,106 @@
         <v>5</v>
       </c>
       <c r="C34" t="n">
-        <v>-0.12326657628229143</v>
+        <v>-0.32188706082796986</v>
       </c>
       <c r="D34" t="n">
-        <v>-0.044756104435859964</v>
+        <v>-0.2385868730930815</v>
       </c>
       <c r="E34" t="n">
-        <v>0.03375436741057145</v>
+        <v>-0.15528668535819315</v>
       </c>
       <c r="F34" t="n">
-        <v>0.1122648392570029</v>
+        <v>-0.07198649762330481</v>
       </c>
       <c r="G34" t="n">
-        <v>0.19077531110343432</v>
+        <v>0.01131369011158355</v>
       </c>
       <c r="H34" t="n">
-        <v>0.26928578294986577</v>
+        <v>0.09461387784647188</v>
       </c>
       <c r="I34" t="n">
-        <v>0.3477962547962973</v>
+        <v>0.17791406558136028</v>
       </c>
       <c r="J34" t="n">
-        <v>0.4263067266427286</v>
+        <v>0.26121425331624853</v>
       </c>
       <c r="K34" t="n">
-        <v>0.5048171984891601</v>
+        <v>0.34451444105113693</v>
       </c>
       <c r="L34" t="n">
-        <v>0.5833276703355916</v>
+        <v>0.4278146287860253</v>
       </c>
       <c r="M34" t="n">
-        <v>0.661838142182023</v>
+        <v>0.5111148165209137</v>
       </c>
       <c r="N34" t="n">
-        <v>0.7403486140284545</v>
+        <v>0.5944150042558021</v>
       </c>
       <c r="O34" t="n">
-        <v>0.818859085874886</v>
+        <v>0.6777151919906905</v>
       </c>
       <c r="P34" t="n">
-        <v>0.897373662889515</v>
+        <v>0.7610153797255789</v>
       </c>
       <c r="Q34" t="n">
-        <v>0.9759526955073328</v>
+        <v>0.8443155674604673</v>
       </c>
       <c r="R34" t="n">
-        <v>1.0546772579339208</v>
+        <v>0.9276157551953557</v>
       </c>
       <c r="S34" t="n">
-        <v>1.13359441371446</v>
+        <v>1.0109159429302441</v>
       </c>
       <c r="T34" t="n">
-        <v>1.2127158509146108</v>
+        <v>1.0942161306651323</v>
       </c>
       <c r="U34" t="n">
-        <v>1.2920178821205142</v>
+        <v>1.1775163184000208</v>
       </c>
       <c r="V34" t="n">
-        <v>1.3714414444387906</v>
+        <v>1.260816600994954</v>
       </c>
       <c r="W34" t="n">
-        <v>1.4508920994965404</v>
+        <v>1.3441938774232907</v>
       </c>
       <c r="X34" t="n">
-        <v>1.5302400334413442</v>
+        <v>1.4278800513457166</v>
       </c>
       <c r="Y34" t="n">
-        <v>1.6093200569412622</v>
+        <v>1.511993536762982</v>
       </c>
       <c r="Z34" t="n">
-        <v>1.6879308371817467</v>
+        <v>1.5964905652809778</v>
       </c>
       <c r="AA34" t="n">
-        <v>1.7634387689733217</v>
+        <v>1.6787690572184044</v>
       </c>
       <c r="AB34" t="n">
-        <v>1.8271200742123175</v>
+        <v>1.7500107210675127</v>
       </c>
       <c r="AC34" t="n">
-        <v>1.872943010893654</v>
+        <v>1.8039632625068807</v>
       </c>
       <c r="AD34" t="n">
-        <v>1.8994415660197954</v>
+        <v>1.8388140773103716</v>
       </c>
       <c r="AE34" t="n">
-        <v>1.9097154556007943</v>
+        <v>1.857190251347189</v>
       </c>
       <c r="AF34" t="n">
-        <v>1.9114301246540921</v>
+        <v>1.8661585605816564</v>
       </c>
       <c r="AG34" t="n">
-        <v>1.9168167472048312</v>
+        <v>1.8772254710735403</v>
       </c>
       <c r="AH34" t="n">
-        <v>1.9426722262855158</v>
+        <v>1.9063371389777175</v>
       </c>
       <c r="AI34" t="n">
-        <v>2.0103591939361793</v>
+        <v>1.973879410544328</v>
       </c>
       <c r="AJ34" t="n">
-        <v>2.1458060112046153</v>
+        <v>2.104677822119022</v>
       </c>
     </row>
     <row r="35">
@@ -36609,106 +36609,106 @@
         <v>5</v>
       </c>
       <c r="C38" t="n">
-        <v>-0.8210319837545976</v>
+        <v>0.41880732905989343</v>
       </c>
       <c r="D38" t="n">
-        <v>-0.8637128548933795</v>
+        <v>0.34640343931213624</v>
       </c>
       <c r="E38" t="n">
-        <v>-0.9063552607076024</v>
+        <v>0.274038014888938</v>
       </c>
       <c r="F38" t="n">
-        <v>-0.9489546814518393</v>
+        <v>0.20171557553572572</v>
       </c>
       <c r="G38" t="n">
-        <v>-0.9915185855816092</v>
+        <v>0.12942865279698024</v>
       </c>
       <c r="H38" t="n">
-        <v>-1.0336731449917993</v>
+        <v>0.0575510747778149</v>
       </c>
       <c r="I38" t="n">
-        <v>-1.0563985620038547</v>
+        <v>0.005102639156783967</v>
       </c>
       <c r="J38" t="n">
-        <v>-1.078470680734625</v>
+        <v>-0.04669249818296148</v>
       </c>
       <c r="K38" t="n">
-        <v>-1.1005770739539855</v>
+        <v>-0.09852191001129759</v>
       </c>
       <c r="L38" t="n">
-        <v>-1.122725820408746</v>
+        <v>-0.1503936750750332</v>
       </c>
       <c r="M38" t="n">
-        <v>-1.1449273927893768</v>
+        <v>-0.20231826606463968</v>
       </c>
       <c r="N38" t="n">
-        <v>-1.1671901671482092</v>
+        <v>-0.25430405903244757</v>
       </c>
       <c r="O38" t="n">
-        <v>-1.1895223776446548</v>
+        <v>-0.30635928813786856</v>
       </c>
       <c r="P38" t="n">
-        <v>-1.211957262923865</v>
+        <v>-0.3584917170305484</v>
       </c>
       <c r="Q38" t="n">
-        <v>-1.23487448373582</v>
+        <v>-0.41070649633417433</v>
       </c>
       <c r="R38" t="n">
-        <v>-1.2587868278050192</v>
+        <v>-0.46301330039923067</v>
       </c>
       <c r="S38" t="n">
-        <v>-1.283995052416965</v>
+        <v>-0.5154208293909669</v>
       </c>
       <c r="T38" t="n">
-        <v>-1.3105765598419632</v>
+        <v>-0.567933954222667</v>
       </c>
       <c r="U38" t="n">
-        <v>-1.3383914168761348</v>
+        <v>-0.620559736096663</v>
       </c>
       <c r="V38" t="n">
-        <v>-1.3670942215902495</v>
+        <v>-0.6733198819158235</v>
       </c>
       <c r="W38" t="n">
-        <v>-1.3970628511573957</v>
+        <v>-0.7276555183757202</v>
       </c>
       <c r="X38" t="n">
-        <v>-1.4380237763934183</v>
+        <v>-0.795537787296412</v>
       </c>
       <c r="Y38" t="n">
-        <v>-1.512156252681912</v>
+        <v>-0.9009058703977117</v>
       </c>
       <c r="Z38" t="n">
-        <v>-1.6257637123171356</v>
+        <v>-1.0510409803495548</v>
       </c>
       <c r="AA38" t="n">
-        <v>-1.7537417317926571</v>
+        <v>-1.2210343280605835</v>
       </c>
       <c r="AB38" t="n">
-        <v>-1.8065610768055989</v>
+        <v>-1.3207701676824142</v>
       </c>
       <c r="AC38" t="n">
-        <v>-1.8248816082204238</v>
+        <v>-1.3895397025733993</v>
       </c>
       <c r="AD38" t="n">
-        <v>-1.7404840619969146</v>
+        <v>-1.3569728652266195</v>
       </c>
       <c r="AE38" t="n">
-        <v>-1.6951062368282757</v>
+        <v>-1.3618745049080527</v>
       </c>
       <c r="AF38" t="n">
-        <v>-1.6782625020672124</v>
+        <v>-1.3900438955825316</v>
       </c>
       <c r="AG38" t="n">
-        <v>-1.6448034393626025</v>
+        <v>-1.391834377550472</v>
       </c>
       <c r="AH38" t="n">
-        <v>-1.5930530559304714</v>
+        <v>-1.3602905707188968</v>
       </c>
       <c r="AI38" t="n">
-        <v>-1.5218006965071362</v>
+        <v>-1.288140286554488</v>
       </c>
       <c r="AJ38" t="n">
-        <v>-1.4299750638371838</v>
+        <v>-1.167468548571665</v>
       </c>
     </row>
     <row r="39">
@@ -36729,106 +36729,106 @@
         <v>5</v>
       </c>
       <c r="C41" t="n">
-        <v>-0.8335436268268754</v>
+        <v>0.3864336375330476</v>
       </c>
       <c r="D41" t="n">
-        <v>-0.8684206968652621</v>
+        <v>0.3223125204745312</v>
       </c>
       <c r="E41" t="n">
-        <v>-0.9032214576427823</v>
+        <v>0.25826771267688164</v>
       </c>
       <c r="F41" t="n">
-        <v>-0.9379646129959641</v>
+        <v>0.19428051030356996</v>
       </c>
       <c r="G41" t="n">
-        <v>-0.9726586489114669</v>
+        <v>0.13034242736793733</v>
       </c>
       <c r="H41" t="n">
-        <v>-1.0069342267796402</v>
+        <v>0.06682280247963446</v>
       </c>
       <c r="I41" t="n">
-        <v>-1.0217750332537798</v>
+        <v>0.022737948985364964</v>
       </c>
       <c r="J41" t="n">
-        <v>-1.0359571055523802</v>
+        <v>-0.020688170333364814</v>
       </c>
       <c r="K41" t="n">
-        <v>-1.0501713151495307</v>
+        <v>-0.06414642695064504</v>
       </c>
       <c r="L41" t="n">
-        <v>-1.0644296503943507</v>
+        <v>-0.10764880921559472</v>
       </c>
       <c r="M41" t="n">
-        <v>-1.0787435785711739</v>
+        <v>-0.15120678441254778</v>
       </c>
       <c r="N41" t="n">
-        <v>-1.0931247410474079</v>
+        <v>-0.19483199390891126</v>
       </c>
       <c r="O41" t="n">
-        <v>-1.107583492579541</v>
+        <v>-0.23853479246117396</v>
       </c>
       <c r="P41" t="n">
-        <v>-1.1221552877159577</v>
+        <v>-0.2823255701390346</v>
       </c>
       <c r="Q41" t="n">
-        <v>-1.1372171945341383</v>
+        <v>-0.32621291993717916</v>
       </c>
       <c r="R41" t="n">
-        <v>-1.1532756193097338</v>
+        <v>-0.3702082421778019</v>
       </c>
       <c r="S41" t="n">
-        <v>-1.1706280699134906</v>
+        <v>-0.4143216939659139</v>
       </c>
       <c r="T41" t="n">
-        <v>-1.1893557799941064</v>
+        <v>-0.4585631463997577</v>
       </c>
       <c r="U41" t="n">
-        <v>-1.2093240367313203</v>
+        <v>-0.502942512323898</v>
       </c>
       <c r="V41" t="n">
-        <v>-1.2301907175711166</v>
+        <v>-0.5474788622410738</v>
       </c>
       <c r="W41" t="n">
-        <v>-1.252351055337186</v>
+        <v>-0.5936135447628359</v>
       </c>
       <c r="X41" t="n">
-        <v>-1.2855477480785198</v>
+        <v>-0.6532977571910767</v>
       </c>
       <c r="Y41" t="n">
-        <v>-1.3519735386319947</v>
+        <v>-0.750455808365622</v>
       </c>
       <c r="Z41" t="n">
-        <v>-1.4579578380315117</v>
+        <v>-0.8923791332540081</v>
       </c>
       <c r="AA41" t="n">
-        <v>-1.5786578884186537</v>
+        <v>-1.054417455862072</v>
       </c>
       <c r="AB41" t="n">
-        <v>-1.6253834586232474</v>
+        <v>-1.1473034848145434</v>
       </c>
       <c r="AC41" t="n">
-        <v>-1.6394608515421025</v>
+        <v>-1.2110169207337553</v>
       </c>
       <c r="AD41" t="n">
-        <v>-1.5528190968182742</v>
+        <v>-1.1753706489189213</v>
       </c>
       <c r="AE41" t="n">
-        <v>-1.5069164097804255</v>
+        <v>-1.1789371982855634</v>
       </c>
       <c r="AF41" t="n">
-        <v>-1.4904531882144494</v>
+        <v>-1.2067617381370122</v>
       </c>
       <c r="AG41" t="n">
-        <v>-1.4570992964199574</v>
+        <v>-1.2080893622209565</v>
       </c>
       <c r="AH41" t="n">
-        <v>-1.403625740718214</v>
+        <v>-1.1744967642374198</v>
       </c>
       <c r="AI41" t="n">
-        <v>-1.3268923653650213</v>
+        <v>-1.0968799337515587</v>
       </c>
       <c r="AJ41" t="n">
-        <v>-1.2235351669837025</v>
+        <v>-0.965141470626743</v>
       </c>
     </row>
     <row r="42">
@@ -36849,106 +36849,106 @@
         <v>5</v>
       </c>
       <c r="C44" t="n">
-        <v>-0.8435529412846974</v>
+        <v>0.3605346843115714</v>
       </c>
       <c r="D44" t="n">
-        <v>-0.8721869704427683</v>
+        <v>0.30303978540444726</v>
       </c>
       <c r="E44" t="n">
-        <v>-0.900714415190926</v>
+        <v>0.2456514709072367</v>
       </c>
       <c r="F44" t="n">
-        <v>-0.929172558231264</v>
+        <v>0.18833245811784544</v>
       </c>
       <c r="G44" t="n">
-        <v>-0.9575706995753532</v>
+        <v>0.13107344702470286</v>
       </c>
       <c r="H44" t="n">
-        <v>-0.9855430922099132</v>
+        <v>0.07424018464108992</v>
       </c>
       <c r="I44" t="n">
-        <v>-0.9940762102537204</v>
+        <v>0.03684619684822954</v>
       </c>
       <c r="J44" t="n">
-        <v>-1.0019462454065848</v>
+        <v>1.1529194631224038E-4</v>
       </c>
       <c r="K44" t="n">
-        <v>-1.009846708105967</v>
+        <v>-0.03664604050212331</v>
       </c>
       <c r="L44" t="n">
-        <v>-1.0177927143828354</v>
+        <v>-0.07345291652804435</v>
       </c>
       <c r="M44" t="n">
-        <v>-1.0257965271966123</v>
+        <v>-0.11031759909087471</v>
       </c>
       <c r="N44" t="n">
-        <v>-1.0338724001667667</v>
+        <v>-0.14725434181008284</v>
       </c>
       <c r="O44" t="n">
-        <v>-1.0420323845274502</v>
+        <v>-0.1842751959198189</v>
       </c>
       <c r="P44" t="n">
-        <v>-1.0503137075496325</v>
+        <v>-0.22139265262582425</v>
       </c>
       <c r="Q44" t="n">
-        <v>-1.0590913631727936</v>
+        <v>-0.2586180588195837</v>
       </c>
       <c r="R44" t="n">
-        <v>-1.0688666525135064</v>
+        <v>-0.29596419560065973</v>
       </c>
       <c r="S44" t="n">
-        <v>-1.0799344839107117</v>
+        <v>-0.33344238562587236</v>
       </c>
       <c r="T44" t="n">
-        <v>-1.0923791561158214</v>
+        <v>-0.3710665001414314</v>
       </c>
       <c r="U44" t="n">
-        <v>-1.1060701326154696</v>
+        <v>-0.4088487333056866</v>
       </c>
       <c r="V44" t="n">
-        <v>-1.1206679143558107</v>
+        <v>-0.4468060465012751</v>
       </c>
       <c r="W44" t="n">
-        <v>-1.1365816186810203</v>
+        <v>-0.48637996587252963</v>
       </c>
       <c r="X44" t="n">
-        <v>-1.1635669254266028</v>
+        <v>-0.5395057331068098</v>
       </c>
       <c r="Y44" t="n">
-        <v>-1.2238273673920614</v>
+        <v>-0.6300957587399516</v>
       </c>
       <c r="Z44" t="n">
-        <v>-1.323713138603014</v>
+        <v>-0.7654496555775718</v>
       </c>
       <c r="AA44" t="n">
-        <v>-1.4385908137194525</v>
+        <v>-0.921123958103264</v>
       </c>
       <c r="AB44" t="n">
-        <v>-1.4804413640773677</v>
+        <v>-1.008530138520248</v>
       </c>
       <c r="AC44" t="n">
-        <v>-1.4911242461994467</v>
+        <v>-1.0681986952620415</v>
       </c>
       <c r="AD44" t="n">
-        <v>-1.4026871246753636</v>
+        <v>-1.0300888758727644</v>
       </c>
       <c r="AE44" t="n">
-        <v>-1.3563645481421474</v>
+        <v>-1.0325873529875733</v>
       </c>
       <c r="AF44" t="n">
-        <v>-1.3402057371322407</v>
+        <v>-1.0601360121805978</v>
       </c>
       <c r="AG44" t="n">
-        <v>-1.3069359820658435</v>
+        <v>-1.0610933499573454</v>
       </c>
       <c r="AH44" t="n">
-        <v>-1.2520838885484107</v>
+        <v>-1.02586171905224</v>
       </c>
       <c r="AI44" t="n">
-        <v>-1.1709657004513314</v>
+        <v>-0.9438716515092166</v>
       </c>
       <c r="AJ44" t="n">
-        <v>-1.0583832495009193</v>
+        <v>-0.8032798082708077</v>
       </c>
     </row>
     <row r="45">
@@ -36974,106 +36974,106 @@
         <v>5</v>
       </c>
       <c r="C48" t="n">
-        <v>-0.11852275184897333</v>
+        <v>-0.326630885261288</v>
       </c>
       <c r="D48" t="n">
-        <v>-0.03978052578869623</v>
+        <v>-0.2435624517402452</v>
       </c>
       <c r="E48" t="n">
-        <v>0.03896170027158082</v>
+        <v>-0.1604940182192025</v>
       </c>
       <c r="F48" t="n">
-        <v>0.11770392633185789</v>
+        <v>-0.0774255846981598</v>
       </c>
       <c r="G48" t="n">
-        <v>0.19644615239213498</v>
+        <v>0.005642848822882934</v>
       </c>
       <c r="H48" t="n">
-        <v>0.27518837845241206</v>
+        <v>0.08871128234392567</v>
       </c>
       <c r="I48" t="n">
-        <v>0.3539306045126891</v>
+        <v>0.1717797158649684</v>
       </c>
       <c r="J48" t="n">
-        <v>0.4326728305729661</v>
+        <v>0.2548481493860111</v>
       </c>
       <c r="K48" t="n">
-        <v>0.5114150566332433</v>
+        <v>0.3379165829070538</v>
       </c>
       <c r="L48" t="n">
-        <v>0.5901572826935203</v>
+        <v>0.42098501642809655</v>
       </c>
       <c r="M48" t="n">
-        <v>0.6688995087537974</v>
+        <v>0.5040534499491394</v>
       </c>
       <c r="N48" t="n">
-        <v>0.7476417348140745</v>
+        <v>0.5871218834701821</v>
       </c>
       <c r="O48" t="n">
-        <v>0.8263839608743517</v>
+        <v>0.6701903169912249</v>
       </c>
       <c r="P48" t="n">
-        <v>0.9051261880288781</v>
+        <v>0.7532587505122675</v>
       </c>
       <c r="Q48" t="n">
-        <v>0.9838908622839224</v>
+        <v>0.8363271840333104</v>
       </c>
       <c r="R48" t="n">
-        <v>1.0627669786291254</v>
+        <v>0.9193956175543531</v>
       </c>
       <c r="S48" t="n">
-        <v>1.1418251509969255</v>
+        <v>1.002464051075396</v>
       </c>
       <c r="T48" t="n">
-        <v>1.2210966983311398</v>
+        <v>1.0855324845964387</v>
       </c>
       <c r="U48" t="n">
-        <v>1.3005736445869651</v>
+        <v>1.1686009181174812</v>
       </c>
       <c r="V48" t="n">
-        <v>1.3802087187309766</v>
+        <v>1.2516732688671233</v>
       </c>
       <c r="W48" t="n">
-        <v>1.4599153547411292</v>
+        <v>1.334880302124441</v>
       </c>
       <c r="X48" t="n">
-        <v>1.5395676916067567</v>
+        <v>1.4184312783859934</v>
       </c>
       <c r="Y48" t="n">
-        <v>1.619000573328572</v>
+        <v>1.5023991388734919</v>
       </c>
       <c r="Z48" t="n">
-        <v>1.6980087809155786</v>
+        <v>1.586706673957675</v>
       </c>
       <c r="AA48" t="n">
-        <v>1.7739509034927514</v>
+        <v>1.668730394266002</v>
       </c>
       <c r="AB48" t="n">
-        <v>1.8380914377617714</v>
+        <v>1.7396426301433738</v>
       </c>
       <c r="AC48" t="n">
-        <v>1.884382997013807</v>
+        <v>1.7931937406649214</v>
       </c>
       <c r="AD48" t="n">
-        <v>1.9113400040384714</v>
+        <v>1.8275858065449688</v>
       </c>
       <c r="AE48" t="n">
-        <v>1.9220386911238634</v>
+        <v>1.8454726301370572</v>
       </c>
       <c r="AF48" t="n">
-        <v>1.9241171000563726</v>
+        <v>1.8539597354337671</v>
       </c>
       <c r="AG48" t="n">
-        <v>1.9297750821209865</v>
+        <v>1.8646043680670192</v>
       </c>
       <c r="AH48" t="n">
-        <v>1.955774298100954</v>
+        <v>1.8934154953077313</v>
       </c>
       <c r="AI48" t="n">
-        <v>2.023438218277954</v>
+        <v>1.9608538060660017</v>
       </c>
       <c r="AJ48" t="n">
-        <v>2.158652122432321</v>
+        <v>2.0918317108913214</v>
       </c>
     </row>
     <row r="49">
@@ -37204,106 +37204,106 @@
         <v>5</v>
       </c>
       <c r="C52" t="n">
-        <v>-0.8516117221056614</v>
+        <v>0.4512516693199687</v>
       </c>
       <c r="D52" t="n">
-        <v>-0.8957307651467562</v>
+        <v>0.3802859514745248</v>
       </c>
       <c r="E52" t="n">
-        <v>-0.9398113428632926</v>
+        <v>0.30935869895363965</v>
       </c>
       <c r="F52" t="n">
-        <v>-0.9838489355098426</v>
+        <v>0.23847443150274072</v>
       </c>
       <c r="G52" t="n">
-        <v>-1.0278510115419262</v>
+        <v>0.1676256806663084</v>
       </c>
       <c r="H52" t="n">
-        <v>-1.0714437428544292</v>
+        <v>0.09718627454945616</v>
       </c>
       <c r="I52" t="n">
-        <v>-1.0956073317687982</v>
+        <v>0.046176010830738634</v>
       </c>
       <c r="J52" t="n">
-        <v>-1.1191176224018815</v>
+        <v>-0.004180954606693599</v>
       </c>
       <c r="K52" t="n">
-        <v>-1.1426621875235556</v>
+        <v>-0.05457219453271643</v>
       </c>
       <c r="L52" t="n">
-        <v>-1.166249105880629</v>
+        <v>-0.10500578769413887</v>
       </c>
       <c r="M52" t="n">
-        <v>-1.1898888501635732</v>
+        <v>-0.155492206781432</v>
       </c>
       <c r="N52" t="n">
-        <v>-1.2135897964247189</v>
+        <v>-0.20603982784692673</v>
       </c>
       <c r="O52" t="n">
-        <v>-1.2373601788234778</v>
+        <v>-0.2566568850500344</v>
       </c>
       <c r="P52" t="n">
-        <v>-1.26120776779996</v>
+        <v>-0.30735114204040104</v>
       </c>
       <c r="Q52" t="n">
-        <v>-1.2852770047160822</v>
+        <v>-0.35812774944171377</v>
       </c>
       <c r="R52" t="n">
-        <v>-1.3101298304439353</v>
+        <v>-0.40899638160445667</v>
       </c>
       <c r="S52" t="n">
-        <v>-1.3362131463441624</v>
+        <v>-0.4599657386938797</v>
       </c>
       <c r="T52" t="n">
-        <v>-1.3637261758911543</v>
+        <v>-0.5110406916232667</v>
       </c>
       <c r="U52" t="n">
-        <v>-1.3926264842140645</v>
+        <v>-0.5622283015949492</v>
       </c>
       <c r="V52" t="n">
-        <v>-1.4226418448456388</v>
+        <v>-0.6135739955683345</v>
       </c>
       <c r="W52" t="n">
-        <v>-1.4541989875498884</v>
+        <v>-0.6668531725099446</v>
       </c>
       <c r="X52" t="n">
-        <v>-1.4970489128625286</v>
+        <v>-0.7338964600205433</v>
       </c>
       <c r="Y52" t="n">
-        <v>-1.5733710830159673</v>
+        <v>-0.8383608543440138</v>
       </c>
       <c r="Z52" t="n">
-        <v>-1.6894448142822203</v>
+        <v>-0.9873200455168182</v>
       </c>
       <c r="AA52" t="n">
-        <v>-1.8201172442615619</v>
+        <v>-1.1557323846567507</v>
       </c>
       <c r="AB52" t="n">
-        <v>-1.8757863768867675</v>
+        <v>-1.253423928967072</v>
       </c>
       <c r="AC52" t="n">
-        <v>-1.8970149883868945</v>
+        <v>-1.319702347700344</v>
       </c>
       <c r="AD52" t="n">
-        <v>-1.8154624072152687</v>
+        <v>-1.2842887020864544</v>
       </c>
       <c r="AE52" t="n">
-        <v>-1.7727207016875792</v>
+        <v>-1.2861536329705998</v>
       </c>
       <c r="AF52" t="n">
-        <v>-1.7581341879079702</v>
+        <v>-1.311336868739493</v>
       </c>
       <c r="AG52" t="n">
-        <v>-1.7263590714056936</v>
+        <v>-1.3105068669579647</v>
       </c>
       <c r="AH52" t="n">
-        <v>-1.6755006604060985</v>
+        <v>-1.2770980276399198</v>
       </c>
       <c r="AI52" t="n">
-        <v>-1.6041052777837765</v>
+        <v>-1.204302605201581</v>
       </c>
       <c r="AJ52" t="n">
-        <v>-1.5108342815505262</v>
+        <v>-1.0847447289493455</v>
       </c>
     </row>
     <row r="53">
@@ -37324,106 +37324,106 @@
         <v>5</v>
       </c>
       <c r="C55" t="n">
-        <v>-0.8636489827346072</v>
+        <v>0.4184035953497912</v>
       </c>
       <c r="D55" t="n">
-        <v>-0.8999410492539227</v>
+        <v>0.35569747477220337</v>
       </c>
       <c r="E55" t="n">
-        <v>-0.9361568065123714</v>
+        <v>0.2930676634554824</v>
       </c>
       <c r="F55" t="n">
-        <v>-0.9723149583464822</v>
+        <v>0.23049545756309953</v>
       </c>
       <c r="G55" t="n">
-        <v>-1.0084239907429136</v>
+        <v>0.1679723711083954</v>
       </c>
       <c r="H55" t="n">
-        <v>-1.0441145650920158</v>
+        <v>0.10586774270102106</v>
       </c>
       <c r="I55" t="n">
-        <v>-1.0603703680470842</v>
+        <v>0.06319788568768042</v>
       </c>
       <c r="J55" t="n">
-        <v>-1.075967436826613</v>
+        <v>0.021186762849879304</v>
       </c>
       <c r="K55" t="n">
-        <v>-1.0915966429046922</v>
+        <v>-0.020856497286472195</v>
       </c>
       <c r="L55" t="n">
-        <v>-1.1072699746304413</v>
+        <v>-0.0629438830704933</v>
       </c>
       <c r="M55" t="n">
-        <v>-1.122998899288193</v>
+        <v>-0.10508686178651758</v>
       </c>
       <c r="N55" t="n">
-        <v>-1.1387950582453554</v>
+        <v>-0.14729707480195242</v>
       </c>
       <c r="O55" t="n">
-        <v>-1.1546688062584174</v>
+        <v>-0.18958487687328637</v>
       </c>
       <c r="P55" t="n">
-        <v>-1.1706305400781163</v>
+        <v>-0.23196065807021835</v>
       </c>
       <c r="Q55" t="n">
-        <v>-1.1868258988367413</v>
+        <v>-0.27443301138743426</v>
       </c>
       <c r="R55" t="n">
-        <v>-1.2038096498791295</v>
+        <v>-0.3170133371471282</v>
       </c>
       <c r="S55" t="n">
-        <v>-1.2220230901124411</v>
+        <v>-0.3597117924543114</v>
       </c>
       <c r="T55" t="n">
-        <v>-1.2416673113016445</v>
+        <v>-0.40253824840722685</v>
       </c>
       <c r="U55" t="n">
-        <v>-1.2627035278226049</v>
+        <v>-0.44550261785043777</v>
       </c>
       <c r="V55" t="n">
-        <v>-1.2848616133972866</v>
+        <v>-0.4886473091063679</v>
       </c>
       <c r="W55" t="n">
-        <v>-1.3085848662052202</v>
+        <v>-0.5337425564269452</v>
       </c>
       <c r="X55" t="n">
-        <v>-1.3436401187310891</v>
+        <v>-0.5926013072111802</v>
       </c>
       <c r="Y55" t="n">
-        <v>-1.4122203173273191</v>
+        <v>-0.688870232100873</v>
       </c>
       <c r="Z55" t="n">
-        <v>-1.520631145623213</v>
+        <v>-0.8296365875536018</v>
       </c>
       <c r="AA55" t="n">
-        <v>-1.643982187435616</v>
+        <v>-0.9901193787534797</v>
       </c>
       <c r="AB55" t="n">
-        <v>-1.6935116223494708</v>
+        <v>-1.080994055191615</v>
       </c>
       <c r="AC55" t="n">
-        <v>-1.7104502330965576</v>
+        <v>-1.1422565180448956</v>
       </c>
       <c r="AD55" t="n">
-        <v>-1.6266075982347608</v>
+        <v>-1.1038093128552968</v>
       </c>
       <c r="AE55" t="n">
-        <v>-1.583298551087422</v>
+        <v>-1.1043880884691233</v>
       </c>
       <c r="AF55" t="n">
-        <v>-1.5690561765149789</v>
+        <v>-1.1292745938087625</v>
       </c>
       <c r="AG55" t="n">
-        <v>-1.5373590949714329</v>
+        <v>-1.128023961929101</v>
       </c>
       <c r="AH55" t="n">
-        <v>-1.4847631380122979</v>
+        <v>-1.0925963855254415</v>
       </c>
       <c r="AI55" t="n">
-        <v>-1.4078890442074843</v>
+        <v>-1.0143448128464838</v>
       </c>
       <c r="AJ55" t="n">
-        <v>-1.303109773574275</v>
+        <v>-0.8837022621271938</v>
       </c>
     </row>
     <row r="56">
@@ -37444,106 +37444,106 @@
         <v>5</v>
       </c>
       <c r="C58" t="n">
-        <v>-0.8732787912377639</v>
+        <v>0.39212513617364936</v>
       </c>
       <c r="D58" t="n">
-        <v>-0.903309276539656</v>
+        <v>0.33602669341034636</v>
       </c>
       <c r="E58" t="n">
-        <v>-0.9332331774316345</v>
+        <v>0.2800348350569567</v>
       </c>
       <c r="F58" t="n">
-        <v>-0.9630877766157937</v>
+        <v>0.22411227841138653</v>
       </c>
       <c r="G58" t="n">
-        <v>-0.9928823741037041</v>
+        <v>0.16824972346206507</v>
       </c>
       <c r="H58" t="n">
-        <v>-1.022251222882085</v>
+        <v>0.11281291722227291</v>
       </c>
       <c r="I58" t="n">
-        <v>-1.0321807970697132</v>
+        <v>0.0768153855732337</v>
       </c>
       <c r="J58" t="n">
-        <v>-1.0414472883663985</v>
+        <v>0.04148093681513737</v>
       </c>
       <c r="K58" t="n">
-        <v>-1.0507442072096018</v>
+        <v>0.0061160605105228805</v>
       </c>
       <c r="L58" t="n">
-        <v>-1.0600866696302913</v>
+        <v>-0.02929435937157722</v>
       </c>
       <c r="M58" t="n">
-        <v>-1.0694869385878891</v>
+        <v>-0.06476258579058645</v>
       </c>
       <c r="N58" t="n">
-        <v>-1.0789592677018651</v>
+        <v>-0.10030287236597356</v>
       </c>
       <c r="O58" t="n">
-        <v>-1.0885157082063692</v>
+        <v>-0.1359272703318885</v>
       </c>
       <c r="P58" t="n">
-        <v>-1.0981687579006418</v>
+        <v>-0.17164827089407286</v>
       </c>
       <c r="Q58" t="n">
-        <v>-1.1080650141332695</v>
+        <v>-0.2074772209440114</v>
       </c>
       <c r="R58" t="n">
-        <v>-1.1187535054272857</v>
+        <v>-0.2434269015812663</v>
       </c>
       <c r="S58" t="n">
-        <v>-1.1306710451270652</v>
+        <v>-0.2795086354626579</v>
       </c>
       <c r="T58" t="n">
-        <v>-1.1440202196300375</v>
+        <v>-0.31573629383439583</v>
       </c>
       <c r="U58" t="n">
-        <v>-1.1587651627094382</v>
+        <v>-0.3521220708548297</v>
       </c>
       <c r="V58" t="n">
-        <v>-1.1746374282386063</v>
+        <v>-0.3887059599367957</v>
       </c>
       <c r="W58" t="n">
-        <v>-1.192093569129487</v>
+        <v>-0.42725406356054696</v>
       </c>
       <c r="X58" t="n">
-        <v>-1.220913083425939</v>
+        <v>-0.47956518496369105</v>
       </c>
       <c r="Y58" t="n">
-        <v>-1.283299704776401</v>
+        <v>-0.5692777343063615</v>
       </c>
       <c r="Z58" t="n">
-        <v>-1.3855802106960085</v>
+        <v>-0.70348982118303</v>
       </c>
       <c r="AA58" t="n">
-        <v>-1.5030741419748603</v>
+        <v>-0.857628974030864</v>
       </c>
       <c r="AB58" t="n">
-        <v>-1.5476918187196347</v>
+        <v>-0.9430501561712513</v>
       </c>
       <c r="AC58" t="n">
-        <v>-1.56119842886429</v>
+        <v>-1.0002998543205386</v>
       </c>
       <c r="AD58" t="n">
-        <v>-1.475523751050356</v>
+        <v>-0.959425801470372</v>
       </c>
       <c r="AE58" t="n">
-        <v>-1.4317608306072982</v>
+        <v>-0.9589756528679441</v>
       </c>
       <c r="AF58" t="n">
-        <v>-1.4177937674005876</v>
+        <v>-0.9836247738641793</v>
       </c>
       <c r="AG58" t="n">
-        <v>-1.3861591138240268</v>
+        <v>-0.982037637906012</v>
       </c>
       <c r="AH58" t="n">
-        <v>-1.3321731200972584</v>
+        <v>-0.9449950718338604</v>
       </c>
       <c r="AI58" t="n">
-        <v>-1.2509160573464522</v>
+        <v>-0.8623785789624075</v>
       </c>
       <c r="AJ58" t="n">
-        <v>-1.1369301671932754</v>
+        <v>-0.7228682886694744</v>
       </c>
     </row>
     <row r="59">
@@ -37569,106 +37569,106 @@
         <v>5</v>
       </c>
       <c r="C62" t="n">
-        <v>-0.11165800671331873</v>
+        <v>-0.3334956303969426</v>
       </c>
       <c r="D62" t="n">
-        <v>-0.03271155764081961</v>
+        <v>-0.2506314198881219</v>
       </c>
       <c r="E62" t="n">
-        <v>0.04623489143167949</v>
+        <v>-0.16776720937930117</v>
       </c>
       <c r="F62" t="n">
-        <v>0.1251813405041786</v>
+        <v>-0.08490299887048047</v>
       </c>
       <c r="G62" t="n">
-        <v>0.2041277895766777</v>
+        <v>-0.002038788361659785</v>
       </c>
       <c r="H62" t="n">
-        <v>0.2830742386491768</v>
+        <v>0.0808254221471609</v>
       </c>
       <c r="I62" t="n">
-        <v>0.36202068772167595</v>
+        <v>0.1636896326559816</v>
       </c>
       <c r="J62" t="n">
-        <v>0.440967136794175</v>
+        <v>0.24655384316480225</v>
       </c>
       <c r="K62" t="n">
-        <v>0.5199135858666741</v>
+        <v>0.329418053673623</v>
       </c>
       <c r="L62" t="n">
-        <v>0.5988600349391733</v>
+        <v>0.4122822641824437</v>
       </c>
       <c r="M62" t="n">
-        <v>0.6778064840116724</v>
+        <v>0.4951464746912644</v>
       </c>
       <c r="N62" t="n">
-        <v>0.7567529330841716</v>
+        <v>0.5780106852000851</v>
       </c>
       <c r="O62" t="n">
-        <v>0.8356993821566707</v>
+        <v>0.6608748957089059</v>
       </c>
       <c r="P62" t="n">
-        <v>0.9146458312291698</v>
+        <v>0.7437391062177265</v>
       </c>
       <c r="Q62" t="n">
-        <v>0.9935954239146859</v>
+        <v>0.8266033167265473</v>
       </c>
       <c r="R62" t="n">
-        <v>1.0726112981446034</v>
+        <v>0.909467527235368</v>
       </c>
       <c r="S62" t="n">
-        <v>1.1517873431097931</v>
+        <v>0.9923317377441887</v>
       </c>
       <c r="T62" t="n">
-        <v>1.2311768210931544</v>
+        <v>1.0751959482530093</v>
       </c>
       <c r="U62" t="n">
-        <v>1.310789655615685</v>
+        <v>1.15806015876183</v>
       </c>
       <c r="V62" t="n">
-        <v>1.3905924314364824</v>
+        <v>1.2409430683213447</v>
       </c>
       <c r="W62" t="n">
-        <v>1.4705083945527413</v>
+        <v>1.3240214429755588</v>
       </c>
       <c r="X62" t="n">
-        <v>1.5504174521997574</v>
+        <v>1.4074653217712667</v>
       </c>
       <c r="Y62" t="n">
-        <v>1.6301561728509228</v>
+        <v>1.4913076864005639</v>
       </c>
       <c r="Z62" t="n">
-        <v>1.7095170182146422</v>
+        <v>1.5754422644264967</v>
       </c>
       <c r="AA62" t="n">
-        <v>1.7858522143420097</v>
+        <v>1.657227400390728</v>
       </c>
       <c r="AB62" t="n">
-        <v>1.8504158510875461</v>
+        <v>1.7278281552742865</v>
       </c>
       <c r="AC62" t="n">
-        <v>1.897146091121979</v>
+        <v>1.7809985155103396</v>
       </c>
       <c r="AD62" t="n">
-        <v>1.9245388628411995</v>
+        <v>1.8149550858931534</v>
       </c>
       <c r="AE62" t="n">
-        <v>1.9356478603663072</v>
+        <v>1.8323770895781308</v>
       </c>
       <c r="AF62" t="n">
-        <v>1.9380845435434084</v>
+        <v>1.840406368081627</v>
       </c>
       <c r="AG62" t="n">
-        <v>1.9440181379439283</v>
+        <v>1.8506473812812378</v>
       </c>
       <c r="AH62" t="n">
-        <v>1.9701756348642754</v>
+        <v>1.879167207415485</v>
       </c>
       <c r="AI62" t="n">
-        <v>2.037841791326004</v>
+        <v>1.9464955430839668</v>
       </c>
       <c r="AJ62" t="n">
-        <v>2.1728591300760476</v>
+        <v>2.0776247032475874</v>
       </c>
     </row>
     <row r="63">
@@ -37799,106 +37799,106 @@
         <v>5</v>
       </c>
       <c r="C66" t="n">
-        <v>-0.8952015895929948</v>
+        <v>0.4972408407343389</v>
       </c>
       <c r="D66" t="n">
-        <v>-0.9405879571547956</v>
+        <v>0.4275424474096011</v>
       </c>
       <c r="E66" t="n">
-        <v>-0.985935859392038</v>
+        <v>0.35788251940942195</v>
       </c>
       <c r="F66" t="n">
-        <v>-1.0312407765592941</v>
+        <v>0.288265576479229</v>
       </c>
       <c r="G66" t="n">
-        <v>-1.0765101771120835</v>
+        <v>0.21868415016350273</v>
       </c>
       <c r="H66" t="n">
-        <v>-1.1213702329452926</v>
+        <v>0.1495120685673566</v>
       </c>
       <c r="I66" t="n">
-        <v>-1.1468011463803673</v>
+        <v>0.09976912936934484</v>
       </c>
       <c r="J66" t="n">
-        <v>-1.1715787615341566</v>
+        <v>0.050679488452618604</v>
       </c>
       <c r="K66" t="n">
-        <v>-1.1963906511765368</v>
+        <v>0.0015555730473016671</v>
       </c>
       <c r="L66" t="n">
-        <v>-1.2212448940543161</v>
+        <v>-0.047610695593414805</v>
       </c>
       <c r="M66" t="n">
-        <v>-1.2461519628579667</v>
+        <v>-0.09682979016000179</v>
       </c>
       <c r="N66" t="n">
-        <v>-1.2711202336398184</v>
+        <v>-0.1461100867047905</v>
       </c>
       <c r="O66" t="n">
-        <v>-1.2961579405592834</v>
+        <v>-0.19545981938719215</v>
       </c>
       <c r="P66" t="n">
-        <v>-1.3212728472660067</v>
+        <v>-0.24488675185685274</v>
       </c>
       <c r="Q66" t="n">
-        <v>-1.3464896123608467</v>
+        <v>-0.29439603473745957</v>
       </c>
       <c r="R66" t="n">
-        <v>-1.3722097183835766</v>
+        <v>-0.3439973423794964</v>
       </c>
       <c r="S66" t="n">
-        <v>-1.3990245034329756</v>
+        <v>-0.3936993749482134</v>
       </c>
       <c r="T66" t="n">
-        <v>-1.4272693623746102</v>
+        <v>-0.4435070033568941</v>
       </c>
       <c r="U66" t="n">
-        <v>-1.4570129377250627</v>
+        <v>-0.4934272888078712</v>
       </c>
       <c r="V66" t="n">
-        <v>-1.488068986400759</v>
+        <v>-0.54359738820517</v>
       </c>
       <c r="W66" t="n">
-        <v>-1.5209251275456377</v>
+        <v>-0.596078162455825</v>
       </c>
       <c r="X66" t="n">
-        <v>-1.5653681570716014</v>
+        <v>-0.6624568468783922</v>
       </c>
       <c r="Y66" t="n">
-        <v>-1.6435882385834848</v>
+        <v>-0.7661424652127349</v>
       </c>
       <c r="Z66" t="n">
-        <v>-1.7618502957219913</v>
+        <v>-0.9140283555926237</v>
       </c>
       <c r="AA66" t="n">
-        <v>-1.8949619794523325</v>
+        <v>-1.0809601378342946</v>
       </c>
       <c r="AB66" t="n">
-        <v>-1.9532567130684682</v>
+        <v>-1.1767187584407754</v>
       </c>
       <c r="AC66" t="n">
-        <v>-1.9772075981568897</v>
+        <v>-1.2406343965656184</v>
       </c>
       <c r="AD66" t="n">
-        <v>-1.8983591945246152</v>
+        <v>-1.2025182439409088</v>
       </c>
       <c r="AE66" t="n">
-        <v>-1.8581637078372775</v>
+        <v>-1.2014986925153264</v>
       </c>
       <c r="AF66" t="n">
-        <v>-1.8458004975452074</v>
+        <v>-1.2238408423803184</v>
       </c>
       <c r="AG66" t="n">
-        <v>-1.8157357185200944</v>
+        <v>-1.2205061434066298</v>
       </c>
       <c r="AH66" t="n">
-        <v>-1.7658595343259929</v>
+        <v>-1.185289608515422</v>
       </c>
       <c r="AI66" t="n">
-        <v>-1.6944780291724308</v>
+        <v>-1.1118117256313216</v>
       </c>
       <c r="AJ66" t="n">
-        <v>-1.5999872284024053</v>
+        <v>-0.9931924781703803</v>
       </c>
     </row>
     <row r="67">
@@ -37919,106 +37919,106 @@
         <v>5</v>
       </c>
       <c r="C69" t="n">
-        <v>-0.9065523757083752</v>
+        <v>0.4637062922505959</v>
       </c>
       <c r="D69" t="n">
-        <v>-0.9440913444471745</v>
+        <v>0.4022470738924919</v>
       </c>
       <c r="E69" t="n">
-        <v>-0.9815540039251068</v>
+        <v>0.34086416479525483</v>
       </c>
       <c r="F69" t="n">
-        <v>-1.0189590579787013</v>
+        <v>0.2795388611223556</v>
       </c>
       <c r="G69" t="n">
-        <v>-1.0563149925946167</v>
+        <v>0.2182626768871354</v>
       </c>
       <c r="H69" t="n">
-        <v>-1.0932524691632026</v>
+        <v>0.15740495069924487</v>
       </c>
       <c r="I69" t="n">
-        <v>-1.1107551743377546</v>
+        <v>0.11598199590538794</v>
       </c>
       <c r="J69" t="n">
-        <v>-1.1275991453367673</v>
+        <v>0.0752177752870706</v>
       </c>
       <c r="K69" t="n">
-        <v>-1.1444752536343303</v>
+        <v>0.03442141737020285</v>
       </c>
       <c r="L69" t="n">
-        <v>-1.161395487579563</v>
+        <v>-0.006419066194334515</v>
       </c>
       <c r="M69" t="n">
-        <v>-1.1783713144567989</v>
+        <v>-0.04731514269087485</v>
       </c>
       <c r="N69" t="n">
-        <v>-1.195414375633445</v>
+        <v>-0.08827845348682593</v>
       </c>
       <c r="O69" t="n">
-        <v>-1.2125350258659906</v>
+        <v>-0.129319353338676</v>
       </c>
       <c r="P69" t="n">
-        <v>-1.2297436552241339</v>
+        <v>-0.1704482323161242</v>
       </c>
       <c r="Q69" t="n">
-        <v>-1.2470680503184295</v>
+        <v>-0.21167368341385634</v>
       </c>
       <c r="R69" t="n">
-        <v>-1.2649051058672232</v>
+        <v>-0.2530071069540664</v>
       </c>
       <c r="S69" t="n">
-        <v>-1.2838382279899676</v>
+        <v>-0.294458660041766</v>
       </c>
       <c r="T69" t="n">
-        <v>-1.3042024855088985</v>
+        <v>-0.33603821377519727</v>
       </c>
       <c r="U69" t="n">
-        <v>-1.3260683802307311</v>
+        <v>-0.377755680998925</v>
       </c>
       <c r="V69" t="n">
-        <v>-1.3492503836818566</v>
+        <v>-0.4197437217977812</v>
       </c>
       <c r="W69" t="n">
-        <v>-1.3742517022198086</v>
+        <v>-0.464053432287714</v>
       </c>
       <c r="X69" t="n">
-        <v>-1.410874386880862</v>
+        <v>-0.5222582897305019</v>
       </c>
       <c r="Y69" t="n">
-        <v>-1.481321912942601</v>
+        <v>-0.6177609882168867</v>
       </c>
       <c r="Z69" t="n">
-        <v>-1.5918858033330778</v>
+        <v>-0.7574713385825251</v>
       </c>
       <c r="AA69" t="n">
-        <v>-1.7176367915414608</v>
+        <v>-0.9164974313185508</v>
       </c>
       <c r="AB69" t="n">
-        <v>-1.7697495171985935</v>
+        <v>-1.0054703321522274</v>
       </c>
       <c r="AC69" t="n">
-        <v>-1.789366533455736</v>
+        <v>-1.0644080894256283</v>
       </c>
       <c r="AD69" t="n">
-        <v>-1.7081844996638345</v>
+        <v>-1.023301926774932</v>
       </c>
       <c r="AE69" t="n">
-        <v>-1.6673806403128766</v>
+        <v>-1.0210427020697428</v>
       </c>
       <c r="AF69" t="n">
-        <v>-1.6553257418035123</v>
+        <v>-1.0431339041848018</v>
       </c>
       <c r="AG69" t="n">
-        <v>-1.62531143650354</v>
+        <v>-1.0394189370563445</v>
       </c>
       <c r="AH69" t="n">
-        <v>-1.57368187825586</v>
+        <v>-1.0022127951901687</v>
       </c>
       <c r="AI69" t="n">
-        <v>-1.4968214382913336</v>
+        <v>-0.9232897595744279</v>
       </c>
       <c r="AJ69" t="n">
-        <v>-1.3908420196617812</v>
+        <v>-0.793570712112602</v>
       </c>
     </row>
     <row r="70">
@@ -38039,106 +38039,106 @@
         <v>5</v>
       </c>
       <c r="C72" t="n">
-        <v>-0.9156330046006795</v>
+        <v>0.43687865346360194</v>
       </c>
       <c r="D72" t="n">
-        <v>-0.9468940542810773</v>
+        <v>0.3820107750788047</v>
       </c>
       <c r="E72" t="n">
-        <v>-0.9780485195515621</v>
+        <v>0.32724948110392116</v>
       </c>
       <c r="F72" t="n">
-        <v>-1.0091336831142272</v>
+        <v>0.272557488836857</v>
       </c>
       <c r="G72" t="n">
-        <v>-1.0401588449806436</v>
+        <v>0.21792549826604152</v>
       </c>
       <c r="H72" t="n">
-        <v>-1.0707582581375306</v>
+        <v>0.16371925640475563</v>
       </c>
       <c r="I72" t="n">
-        <v>-1.081918396703665</v>
+        <v>0.12895228913422224</v>
       </c>
       <c r="J72" t="n">
-        <v>-1.092415452378856</v>
+        <v>0.09484840475463197</v>
       </c>
       <c r="K72" t="n">
-        <v>-1.102942935600566</v>
+        <v>0.06071409282852344</v>
       </c>
       <c r="L72" t="n">
-        <v>-1.1135159623997606</v>
+        <v>0.02653423732492933</v>
       </c>
       <c r="M72" t="n">
-        <v>-1.1241467957358648</v>
+        <v>-0.0077034247155737395</v>
       </c>
       <c r="N72" t="n">
-        <v>-1.134849689228347</v>
+        <v>-0.04201314691245482</v>
       </c>
       <c r="O72" t="n">
-        <v>-1.145636694111357</v>
+        <v>-0.07640698049986366</v>
       </c>
       <c r="P72" t="n">
-        <v>-1.156520301590636</v>
+        <v>-0.11089741668354192</v>
       </c>
       <c r="Q72" t="n">
-        <v>-1.1675308006844967</v>
+        <v>-0.14549580235497456</v>
       </c>
       <c r="R72" t="n">
-        <v>-1.1790614158541413</v>
+        <v>-0.1802149186137233</v>
       </c>
       <c r="S72" t="n">
-        <v>-1.1916892076355619</v>
+        <v>-0.21506608811660877</v>
       </c>
       <c r="T72" t="n">
-        <v>-1.2057489840163305</v>
+        <v>-0.2500631821098406</v>
       </c>
       <c r="U72" t="n">
-        <v>-1.2213127342352665</v>
+        <v>-0.2852183947517689</v>
       </c>
       <c r="V72" t="n">
-        <v>-1.2381955015067354</v>
+        <v>-0.3206607886718712</v>
       </c>
       <c r="W72" t="n">
-        <v>-1.2569129619591461</v>
+        <v>-0.3584336481532263</v>
       </c>
       <c r="X72" t="n">
-        <v>-1.2872793707282715</v>
+        <v>-0.410099444012191</v>
       </c>
       <c r="Y72" t="n">
-        <v>-1.3515088524298953</v>
+        <v>-0.49905580662021</v>
       </c>
       <c r="Z72" t="n">
-        <v>-1.4559142094219488</v>
+        <v>-0.6322257249744474</v>
       </c>
       <c r="AA72" t="n">
-        <v>-1.5757766412127638</v>
+        <v>-0.7849272661059572</v>
       </c>
       <c r="AB72" t="n">
-        <v>-1.6229437605026957</v>
+        <v>-0.8684715911213902</v>
       </c>
       <c r="AC72" t="n">
-        <v>-1.6390936816948143</v>
+        <v>-0.9234270437136376</v>
       </c>
       <c r="AD72" t="n">
-        <v>-1.5560447437752112</v>
+        <v>-0.8799288730421528</v>
       </c>
       <c r="AE72" t="n">
-        <v>-1.5147541862933571</v>
+        <v>-0.8766779097132771</v>
       </c>
       <c r="AF72" t="n">
-        <v>-1.5029459372101583</v>
+        <v>-0.8985683536283903</v>
       </c>
       <c r="AG72" t="n">
-        <v>-1.472972010890298</v>
+        <v>-0.8945491719761177</v>
       </c>
       <c r="AH72" t="n">
-        <v>-1.4199397533997553</v>
+        <v>-0.8557513445299669</v>
       </c>
       <c r="AI72" t="n">
-        <v>-1.3386961655864575</v>
+        <v>-0.7724721867289147</v>
       </c>
       <c r="AJ72" t="n">
-        <v>-1.2235258526692838</v>
+        <v>-0.6338732992663811</v>
       </c>
     </row>
   </sheetData>

</xml_diff>